<commit_message>
Update Excel sample and docs and vba add-in
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -13,15 +13,13 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Critical temperature of R410A:</t>
   </si>
@@ -114,9 +112,6 @@
     <t>Pa-s</t>
   </si>
   <si>
-    <t>CAS code of Water:</t>
-  </si>
-  <si>
     <t>Example of an error:</t>
   </si>
   <si>
@@ -127,13 +122,34 @@
   </si>
   <si>
     <t>Expected value</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>Nitrogen</t>
+  </si>
+  <si>
+    <t>Argon</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>Dewpoint of dry air at 1 atm:</t>
+  </si>
+  <si>
+    <t>Mixture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +168,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -185,6 +210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -257,121 +283,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>6.1220371526289217E-4</c:v>
+                  <c:v>6.1220262250698829E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.021255883981318</c:v>
+                  <c:v>42.021255884023319</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83.914144952811796</c:v>
+                  <c:v>83.914144952255299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>125.73397341921785</c:v>
+                  <c:v>125.73397341873977</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>167.5330355872081</c:v>
+                  <c:v>167.53303558684075</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>209.34176132668705</c:v>
+                  <c:v>209.34176132638896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>251.18035191394253</c:v>
+                  <c:v>251.18035191373392</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>293.06519282229988</c:v>
+                  <c:v>293.06519282209621</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>335.01235325254447</c:v>
+                  <c:v>335.01235325239014</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>377.03938647776687</c:v>
+                  <c:v>377.03938647762016</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>419.16616289289658</c:v>
+                  <c:v>419.16616289276845</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>461.4151895343303</c:v>
+                  <c:v>461.41518953422172</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>503.81169242147121</c:v>
+                  <c:v>503.81169242137508</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>546.38362438115269</c:v>
+                  <c:v>546.38362438106753</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>589.16169048823679</c:v>
+                  <c:v>589.16169048816187</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>632.17944178056644</c:v>
+                  <c:v>632.17944178050175</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>675.47346558322408</c:v>
+                  <c:v>675.47346558316849</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>719.08369096295746</c:v>
+                  <c:v>719.08369096290494</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>763.05382639583047</c:v>
+                  <c:v>763.05382639578045</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>807.43195145025493</c:v>
+                  <c:v>807.43195145020456</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>852.27129446018387</c:v>
+                  <c:v>852.27129446014476</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>897.63124444416621</c:v>
+                  <c:v>897.63124444412767</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>943.5786700422118</c:v>
+                  <c:v>943.57867004221146</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>990.18965507747453</c:v>
+                  <c:v>990.1896550774411</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1037.5518165790263</c:v>
+                  <c:v>1037.551816578999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1085.7674588110503</c:v>
+                  <c:v>1085.7674588110201</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1134.9579569891296</c:v>
+                  <c:v>1134.9579569891007</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1185.2699943566126</c:v>
+                  <c:v>1185.2699943565901</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1236.8846659592693</c:v>
+                  <c:v>1236.8846659592452</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1290.0311497479681</c:v>
+                  <c:v>1290.0311497479454</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1345.0079264161157</c:v>
+                  <c:v>1345.0079264160959</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1402.2171260009688</c:v>
+                  <c:v>1402.2171260009461</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1462.2236463970917</c:v>
+                  <c:v>1462.2236463970723</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1525.8683270564179</c:v>
+                  <c:v>1525.8683270550459</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1594.5289922369011</c:v>
+                  <c:v>1594.5289922362745</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1670.8899067287161</c:v>
+                  <c:v>1670.8899067277875</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1761.6646205625962</c:v>
+                  <c:v>1761.6646205355191</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1890.6872488661784</c:v>
+                  <c:v>1890.6872488661456</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2060.0042388923648</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -383,121 +409,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0.61165477790576328</c:v>
+                  <c:v>0.61165479346263607</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2281989260750077</c:v>
+                  <c:v>1.2281989137439591</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3393181837875359</c:v>
+                  <c:v>2.3393181982305578</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2469708407183706</c:v>
+                  <c:v>4.2469708476789396</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3849380739551265</c:v>
+                  <c:v>7.3849380690927697</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.351945840547332</c:v>
+                  <c:v>12.351945836928898</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.946434302277851</c:v>
+                  <c:v>19.946434308589296</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.200930025942377</c:v>
+                  <c:v>31.200930027430044</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.414474030019207</c:v>
+                  <c:v>47.414474029828604</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.181765814537528</c:v>
+                  <c:v>70.181765815372145</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.41799666002106</c:v>
+                  <c:v>101.41799665916226</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.37871294940228</c:v>
+                  <c:v>143.37871294902544</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198.67442047934145</c:v>
+                  <c:v>198.6744204783304</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>270.27997678530858</c:v>
+                  <c:v>270.27997678512435</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>361.53909939988046</c:v>
+                  <c:v>361.53909939990245</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>476.16453797031113</c:v>
+                  <c:v>476.16453796936935</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>618.23462142577796</c:v>
+                  <c:v>618.23462142627261</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>792.18700698190401</c:v>
+                  <c:v>792.18700698253531</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1002.8105360782905</c:v>
+                  <c:v>1002.8105360782382</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1255.2361551605081</c:v>
+                  <c:v>1255.2361551608849</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1554.9279004667762</c:v>
+                  <c:v>1554.9279004671425</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1907.6749935324397</c:v>
+                  <c:v>1907.6749935317039</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2319.5861701998538</c:v>
+                  <c:v>2319.5861702587372</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2797.0874969297211</c:v>
+                  <c:v>2797.0874969298998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3346.9251442691252</c:v>
+                  <c:v>3346.9251442694003</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3976.1749306524707</c:v>
+                  <c:v>3976.1749306524598</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4692.260992299709</c:v>
+                  <c:v>4692.2609922994561</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5502.986783014605</c:v>
+                  <c:v>5502.9867830146577</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6416.582909532026</c:v>
+                  <c:v>6416.5829095316267</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7441.7783444212137</c:v>
+                  <c:v>7441.7783444209954</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8587.9049408353676</c:v>
+                  <c:v>8587.9049408353076</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9865.0512111820826</c:v>
+                  <c:v>9865.0512111816915</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11284.292927464725</c:v>
+                  <c:v>11284.292927464572</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12858.051600018429</c:v>
+                  <c:v>12858.051600204713</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14600.677371948063</c:v>
+                  <c:v>14600.677372002207</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16529.415139004064</c:v>
+                  <c:v>16529.415139051285</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18666.006645644644</c:v>
+                  <c:v>18666.006646276048</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21043.56314746592</c:v>
+                  <c:v>21043.563147465924</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22061.328131850038</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -524,121 +550,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>2500.9151916490418</c:v>
+                  <c:v>2500.9151916490428</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2519.2083189072159</c:v>
+                  <c:v>2519.2083189072168</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2537.4334043725835</c:v>
+                  <c:v>2537.4334043725839</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2555.545203294766</c:v>
+                  <c:v>2555.5452032947665</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2573.510322374003</c:v>
+                  <c:v>2573.5103223740039</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2591.2888878672011</c:v>
+                  <c:v>2591.288887867202</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2608.834872217727</c:v>
+                  <c:v>2608.8348722177279</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2626.0964008315314</c:v>
+                  <c:v>2626.0964008315277</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2643.0158813452254</c:v>
+                  <c:v>2643.0158813452158</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2659.5300141957478</c:v>
+                  <c:v>2659.5300141957387</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2675.5698844194635</c:v>
+                  <c:v>2675.5698844194603</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2691.0613426859572</c:v>
+                  <c:v>2691.0613426859577</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2705.9257657931835</c:v>
+                  <c:v>2705.9257657931848</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2720.0811051450501</c:v>
+                  <c:v>2720.0811051450514</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2733.4429731737555</c:v>
+                  <c:v>2733.4429731737559</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2745.9254514300796</c:v>
+                  <c:v>2745.9254514300715</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2757.4413489921203</c:v>
+                  <c:v>2757.441348992098</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2767.901762261462</c:v>
+                  <c:v>2767.9017622614292</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2777.2149260216215</c:v>
+                  <c:v>2777.2149260215924</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2785.2844447620487</c:v>
+                  <c:v>2785.2844447620337</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2792.0070226267294</c:v>
+                  <c:v>2792.0070226267262</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2797.2697683428019</c:v>
+                  <c:v>2797.2697683428046</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2800.9470527725616</c:v>
+                  <c:v>2800.9470527725671</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2802.8967584010438</c:v>
+                  <c:v>2802.8967584010479</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2802.9556046252342</c:v>
+                  <c:v>2802.9556046252392</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2800.9330729758321</c:v>
+                  <c:v>2800.9330729758371</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2796.6032203853524</c:v>
+                  <c:v>2796.6032203853574</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2789.6932193000084</c:v>
+                  <c:v>2789.6932193000157</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2779.8667305294553</c:v>
+                  <c:v>2779.8667305294593</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2766.6990506391335</c:v>
+                  <c:v>2766.6990506391412</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2749.6387614002501</c:v>
+                  <c:v>2749.6387614002556</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2727.9458789653868</c:v>
+                  <c:v>2727.9458789653931</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2700.5857692409354</c:v>
+                  <c:v>2700.5857692409404</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2666.0311405571751</c:v>
+                  <c:v>2666.031140557182</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2621.8455755251834</c:v>
+                  <c:v>2621.8455755251885</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2563.6367109445368</c:v>
+                  <c:v>2563.6367109445987</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2481.4924833322702</c:v>
+                  <c:v>2481.4924833359923</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2334.5182916068165</c:v>
+                  <c:v>2334.5182916067993</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2110.5585219387103</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,121 +676,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0.61165477790576328</c:v>
+                  <c:v>0.61165479346263607</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2281989260750077</c:v>
+                  <c:v>1.2281989137439591</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3393181837875359</c:v>
+                  <c:v>2.3393181982305578</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2469708407183706</c:v>
+                  <c:v>4.2469708476789396</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3849380739551265</c:v>
+                  <c:v>7.3849380690927697</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.351945840547332</c:v>
+                  <c:v>12.351945836928898</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.946434302277851</c:v>
+                  <c:v>19.946434308589296</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.200930025942377</c:v>
+                  <c:v>31.200930027430044</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.414474030019207</c:v>
+                  <c:v>47.414474029828604</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.181765814537528</c:v>
+                  <c:v>70.181765815372145</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.41799666002106</c:v>
+                  <c:v>101.41799665916226</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.37871294940228</c:v>
+                  <c:v>143.37871294902544</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198.67442047934145</c:v>
+                  <c:v>198.6744204783304</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>270.27997678530858</c:v>
+                  <c:v>270.27997678512435</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>361.53909939988046</c:v>
+                  <c:v>361.53909939990245</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>476.16453797031113</c:v>
+                  <c:v>476.16453796936935</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>618.23462142577796</c:v>
+                  <c:v>618.23462142627261</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>792.18700698190401</c:v>
+                  <c:v>792.18700698253531</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1002.8105360782905</c:v>
+                  <c:v>1002.8105360782382</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1255.2361551605081</c:v>
+                  <c:v>1255.2361551608849</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1554.9279004667762</c:v>
+                  <c:v>1554.9279004671425</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1907.6749935324397</c:v>
+                  <c:v>1907.6749935317039</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2319.5861701998538</c:v>
+                  <c:v>2319.5861702587372</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2797.0874969297211</c:v>
+                  <c:v>2797.0874969298998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3346.9251442691252</c:v>
+                  <c:v>3346.9251442694003</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3976.1749306524707</c:v>
+                  <c:v>3976.1749306524598</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4692.260992299709</c:v>
+                  <c:v>4692.2609922994561</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5502.986783014605</c:v>
+                  <c:v>5502.9867830146577</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6416.582909532026</c:v>
+                  <c:v>6416.5829095316267</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7441.7783444212137</c:v>
+                  <c:v>7441.7783444209954</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8587.9049408353676</c:v>
+                  <c:v>8587.9049408353076</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9865.0512111820826</c:v>
+                  <c:v>9865.0512111816915</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11284.292927464725</c:v>
+                  <c:v>11284.292927464572</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12858.051600018429</c:v>
+                  <c:v>12858.051600204713</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14600.677371948063</c:v>
+                  <c:v>14600.677372002207</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16529.415139004064</c:v>
+                  <c:v>16529.415139051285</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18666.006645644644</c:v>
+                  <c:v>18666.006646276048</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21043.56314746592</c:v>
+                  <c:v>21043.563147465924</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22061.328131850038</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -779,11 +805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169266176"/>
-        <c:axId val="138871936"/>
+        <c:axId val="123193984"/>
+        <c:axId val="123753216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169266176"/>
+        <c:axId val="123193984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,12 +837,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138871936"/>
+        <c:crossAx val="123753216"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="138871936"/>
+        <c:axId val="123753216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -845,7 +871,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169266176"/>
+        <c:crossAx val="123193984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -906,7 +932,9 @@
       <sheetName val="Sheet3"/>
     </sheetNames>
     <definedNames>
+      <definedName name="MixtureString"/>
       <definedName name="Props"/>
+      <definedName name="Props1"/>
       <definedName name="Props1SI"/>
       <definedName name="PropsSI"/>
     </definedNames>
@@ -914,29 +942,6 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sample calcs"/>
-      <sheetName val="Water saturation table"/>
-      <sheetName val="Sheet3"/>
-      <sheetName val="CoolProp"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="Props"/>
-      <definedName name="Props1"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1230,16 +1235,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1265,10 +1270,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1278,9 +1283,9 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="str">
+      <c r="C6" s="4">
         <f>[1]!Props1SI("R410A","Tcrit")</f>
-        <v>Your input name [Tcrit] is not valid in get_parameter_index (names are case sensitive)</v>
+        <v>344.49400000000003</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,9 +1295,9 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="str">
+      <c r="C7" s="4">
         <f>[1]!Props1SI("Propane","rhocrit")</f>
-        <v>Your input name [rhocrit] is not valid in get_parameter_index (names are case sensitive)</v>
+        <v>220.47810000000004</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1316,7 +1321,7 @@
       </c>
       <c r="C9" s="4">
         <f>[1]!PropsSI("T","P",101325,"Q",0,"HEOS::Water")-273.15</f>
-        <v>99.97429584768787</v>
+        <v>99.97429584768804</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,7 +1333,7 @@
       </c>
       <c r="C10" s="4">
         <f>[1]!PropsSI("T","P",101325,"Q",0,"REFPROP::Water")-273.15</f>
-        <v>99.974295847697647</v>
+        <v>99.974295847697988</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,29 +1341,71 @@
         <v>21</v>
       </c>
       <c r="C11" s="4" t="str">
-        <f>[1]!Props1SI("Water","CAS")</f>
-        <v>Your input name [CAS] is not valid in get_parameter_index (names are case sensitive)</v>
+        <f>[1]!Props1SI("A","B")</f>
+        <v>Neither input to Props1SI [A,B] is a valid fluid</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="str">
-        <f>[1]!Props1SI("A","B")</f>
-        <v>Your input name [B] is not valid in get_parameter_index (names are case sensitive)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="4" t="str">
-        <f>[1]!PropsSI("V","T",300,"P",101.325,"BRINE::EG[20%]")</f>
-        <v>Your input name [V] is not valid in get_parameter_index (names are case sensitive)</v>
+      <c r="C12" s="4">
+        <f>[1]!PropsSI("V","T",300,"P",101.325,"INCOMP::MEG[0.2]")</f>
+        <v>1.38142216644215E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>0.78090000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>0.20949999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>9.2999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19">
+        <v>3.8999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <f>[1]!PropsSI("T","P",101325,"Q",0,"HEOS::"&amp;[1]!MixtureString(A16:A19,B16:B19))</f>
+        <v>78.650190680028572</v>
       </c>
     </row>
   </sheetData>
@@ -1460,24 +1507,24 @@
         <v>273.16000009999999</v>
       </c>
       <c r="C6">
-        <f>[2]!Props("P","T",B6,"Q",0,"Water")</f>
-        <v>0.61165477790576328</v>
+        <f>[1]!Props("P","T",B6,"Q",0,"Water")</f>
+        <v>0.61165479346263607</v>
       </c>
       <c r="D6">
-        <f>[2]!Props("D","T",B6,"Q",0,"Water")</f>
-        <v>999.79252003842566</v>
+        <f>[1]!Props("D","T",B6,"Q",0,"Water")</f>
+        <v>999.79252003792112</v>
       </c>
       <c r="E6">
-        <f>[2]!Props("D","T",B6,"Q",1,"Water")</f>
-        <v>4.8545757582901831E-3</v>
+        <f>[1]!Props("D","T",B6,"Q",1,"Water")</f>
+        <v>4.854575758285436E-3</v>
       </c>
       <c r="F6">
-        <f>[2]!Props("H","T",B6,"Q",0,"Water")</f>
-        <v>6.1220371526289217E-4</v>
+        <f>[1]!Props("H","T",B6,"Q",0,"Water")</f>
+        <v>6.1220262250698829E-4</v>
       </c>
       <c r="G6">
-        <f>[2]!Props("H","T",B6,"Q",1,"Water")</f>
-        <v>2500.9151916490418</v>
+        <f>[1]!Props("H","T",B6,"Q",1,"Water")</f>
+        <v>2500.9151916490428</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1489,24 +1536,24 @@
         <v>283.14999999999998</v>
       </c>
       <c r="C7">
-        <f>[2]!Props("P","T",B7,"Q",0,"Water")</f>
-        <v>1.2281989260750077</v>
+        <f>[1]!Props("P","T",B7,"Q",0,"Water")</f>
+        <v>1.2281989137439591</v>
       </c>
       <c r="D7">
-        <f>[2]!Props("D","T",B7,"Q",0,"Water")</f>
-        <v>999.65462464159361</v>
+        <f>[1]!Props("D","T",B7,"Q",0,"Water")</f>
+        <v>999.65462464124357</v>
       </c>
       <c r="E7">
-        <f>[2]!Props("D","T",B7,"Q",1,"Water")</f>
-        <v>9.4070520080230726E-3</v>
+        <f>[1]!Props("D","T",B7,"Q",1,"Water")</f>
+        <v>9.407052008015733E-3</v>
       </c>
       <c r="F7">
         <f>[1]!Props("H","T",B7,"Q",0,"Water")</f>
-        <v>42.021255883981318</v>
+        <v>42.021255884023319</v>
       </c>
       <c r="G7">
-        <f>[2]!Props("H","T",B7,"Q",1,"Water")</f>
-        <v>2519.2083189072159</v>
+        <f>[1]!Props("H","T",B7,"Q",1,"Water")</f>
+        <v>2519.2083189072168</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1518,24 +1565,24 @@
         <v>293.14999999999998</v>
       </c>
       <c r="C8">
-        <f>[2]!Props("P","T",B8,"Q",0,"Water")</f>
-        <v>2.3393181837875359</v>
+        <f>[1]!Props("P","T",B8,"Q",0,"Water")</f>
+        <v>2.3393181982305578</v>
       </c>
       <c r="D8">
-        <f>[2]!Props("D","T",B8,"Q",0,"Water")</f>
-        <v>998.16180134317437</v>
+        <f>[1]!Props("D","T",B8,"Q",0,"Water")</f>
+        <v>998.16180134293222</v>
       </c>
       <c r="E8">
-        <f>[2]!Props("D","T",B8,"Q",1,"Water")</f>
-        <v>1.7314008205457157E-2</v>
+        <f>[1]!Props("D","T",B8,"Q",1,"Water")</f>
+        <v>1.7314008205447751E-2</v>
       </c>
       <c r="F8">
-        <f>[2]!Props("H","T",B8,"Q",0,"Water")</f>
-        <v>83.914144952811796</v>
+        <f>[1]!Props("H","T",B8,"Q",0,"Water")</f>
+        <v>83.914144952255299</v>
       </c>
       <c r="G8">
-        <f>[2]!Props("H","T",B8,"Q",1,"Water")</f>
-        <v>2537.4334043725835</v>
+        <f>[1]!Props("H","T",B8,"Q",1,"Water")</f>
+        <v>2537.4334043725839</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1547,24 +1594,24 @@
         <v>303.14999999999998</v>
       </c>
       <c r="C9">
-        <f>[2]!Props("P","T",B9,"Q",0,"Water")</f>
-        <v>4.2469708407183706</v>
+        <f>[1]!Props("P","T",B9,"Q",0,"Water")</f>
+        <v>4.2469708476789396</v>
       </c>
       <c r="D9">
-        <f>[2]!Props("D","T",B9,"Q",0,"Water")</f>
-        <v>995.60617747384663</v>
+        <f>[1]!Props("D","T",B9,"Q",0,"Water")</f>
+        <v>995.60617747366496</v>
       </c>
       <c r="E9">
-        <f>[2]!Props("D","T",B9,"Q",1,"Water")</f>
-        <v>3.0415211808982323E-2</v>
+        <f>[1]!Props("D","T",B9,"Q",1,"Water")</f>
+        <v>3.0415211808968497E-2</v>
       </c>
       <c r="F9">
-        <f>[2]!Props("H","T",B9,"Q",0,"Water")</f>
-        <v>125.73397341921785</v>
+        <f>[1]!Props("H","T",B9,"Q",0,"Water")</f>
+        <v>125.73397341873977</v>
       </c>
       <c r="G9">
-        <f>[2]!Props("H","T",B9,"Q",1,"Water")</f>
-        <v>2555.545203294766</v>
+        <f>[1]!Props("H","T",B9,"Q",1,"Water")</f>
+        <v>2555.5452032947665</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1576,24 +1623,24 @@
         <v>313.14999999999998</v>
       </c>
       <c r="C10">
-        <f>[2]!Props("P","T",B10,"Q",0,"Water")</f>
-        <v>7.3849380739551265</v>
+        <f>[1]!Props("P","T",B10,"Q",0,"Water")</f>
+        <v>7.3849380690927697</v>
       </c>
       <c r="D10">
-        <f>[2]!Props("D","T",B10,"Q",0,"Water")</f>
-        <v>992.17511534129721</v>
+        <f>[1]!Props("D","T",B10,"Q",0,"Water")</f>
+        <v>992.17511534115829</v>
       </c>
       <c r="E10">
-        <f>[2]!Props("D","T",B10,"Q",1,"Water")</f>
-        <v>5.1242255801689097E-2</v>
+        <f>[1]!Props("D","T",B10,"Q",1,"Water")</f>
+        <v>5.124225580167082E-2</v>
       </c>
       <c r="F10">
-        <f>[2]!Props("H","T",B10,"Q",0,"Water")</f>
-        <v>167.5330355872081</v>
+        <f>[1]!Props("H","T",B10,"Q",0,"Water")</f>
+        <v>167.53303558684075</v>
       </c>
       <c r="G10">
-        <f>[2]!Props("H","T",B10,"Q",1,"Water")</f>
-        <v>2573.510322374003</v>
+        <f>[1]!Props("H","T",B10,"Q",1,"Water")</f>
+        <v>2573.5103223740039</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1605,24 +1652,24 @@
         <v>323.14999999999998</v>
       </c>
       <c r="C11">
-        <f>[2]!Props("P","T",B11,"Q",0,"Water")</f>
-        <v>12.351945840547332</v>
+        <f>[1]!Props("P","T",B11,"Q",0,"Water")</f>
+        <v>12.351945836928898</v>
       </c>
       <c r="D11">
-        <f>[2]!Props("D","T",B11,"Q",0,"Water")</f>
-        <v>987.9962106111717</v>
+        <f>[1]!Props("D","T",B11,"Q",0,"Water")</f>
+        <v>987.99621061106234</v>
       </c>
       <c r="E11">
-        <f>[2]!Props("D","T",B11,"Q",1,"Water")</f>
-        <v>8.3146842800445916E-2</v>
+        <f>[1]!Props("D","T",B11,"Q",1,"Water")</f>
+        <v>8.3146842800420256E-2</v>
       </c>
       <c r="F11">
-        <f>[2]!Props("H","T",B11,"Q",0,"Water")</f>
-        <v>209.34176132668705</v>
+        <f>[1]!Props("H","T",B11,"Q",0,"Water")</f>
+        <v>209.34176132638896</v>
       </c>
       <c r="G11">
-        <f>[2]!Props("H","T",B11,"Q",1,"Water")</f>
-        <v>2591.2888878672011</v>
+        <f>[1]!Props("H","T",B11,"Q",1,"Water")</f>
+        <v>2591.288887867202</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1634,24 +1681,24 @@
         <v>333.15</v>
       </c>
       <c r="C12">
-        <f>[2]!Props("P","T",B12,"Q",0,"Water")</f>
-        <v>19.946434302277851</v>
+        <f>[1]!Props("P","T",B12,"Q",0,"Water")</f>
+        <v>19.946434308589296</v>
       </c>
       <c r="D12">
-        <f>[2]!Props("D","T",B12,"Q",0,"Water")</f>
-        <v>983.16021717833303</v>
+        <f>[1]!Props("D","T",B12,"Q",0,"Water")</f>
+        <v>983.16021717825356</v>
       </c>
       <c r="E12">
-        <f>[2]!Props("D","T",B12,"Q",1,"Water")</f>
-        <v>0.13042522259659625</v>
+        <f>[1]!Props("D","T",B12,"Q",1,"Water")</f>
+        <v>0.1304252225965658</v>
       </c>
       <c r="F12">
-        <f>[2]!Props("H","T",B12,"Q",0,"Water")</f>
-        <v>251.18035191394253</v>
+        <f>[1]!Props("H","T",B12,"Q",0,"Water")</f>
+        <v>251.18035191373392</v>
       </c>
       <c r="G12">
-        <f>[2]!Props("H","T",B12,"Q",1,"Water")</f>
-        <v>2608.834872217727</v>
+        <f>[1]!Props("H","T",B12,"Q",1,"Water")</f>
+        <v>2608.8348722177279</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1663,24 +1710,24 @@
         <v>343.15</v>
       </c>
       <c r="C13">
-        <f>[2]!Props("P","T",B13,"Q",0,"Water")</f>
-        <v>31.200930025942377</v>
+        <f>[1]!Props("P","T",B13,"Q",0,"Water")</f>
+        <v>31.200930027430044</v>
       </c>
       <c r="D13">
-        <f>[2]!Props("D","T",B13,"Q",0,"Water")</f>
-        <v>977.73365598192868</v>
+        <f>[1]!Props("D","T",B13,"Q",0,"Water")</f>
+        <v>977.73365598186456</v>
       </c>
       <c r="E13">
-        <f>[2]!Props("D","T",B13,"Q",1,"Water")</f>
-        <v>0.19843073794182545</v>
+        <f>[1]!Props("D","T",B13,"Q",1,"Water")</f>
+        <v>0.19843073794194227</v>
       </c>
       <c r="F13">
-        <f>[2]!Props("H","T",B13,"Q",0,"Water")</f>
-        <v>293.06519282229988</v>
+        <f>[1]!Props("H","T",B13,"Q",0,"Water")</f>
+        <v>293.06519282209621</v>
       </c>
       <c r="G13">
-        <f>[2]!Props("H","T",B13,"Q",1,"Water")</f>
-        <v>2626.0964008315314</v>
+        <f>[1]!Props("H","T",B13,"Q",1,"Water")</f>
+        <v>2626.0964008315277</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1692,24 +1739,24 @@
         <v>353.15</v>
       </c>
       <c r="C14">
-        <f>[2]!Props("P","T",B14,"Q",0,"Water")</f>
-        <v>47.414474030019207</v>
+        <f>[1]!Props("P","T",B14,"Q",0,"Water")</f>
+        <v>47.414474029828604</v>
       </c>
       <c r="D14">
-        <f>[2]!Props("D","T",B14,"Q",0,"Water")</f>
-        <v>971.76621871051145</v>
+        <f>[1]!Props("D","T",B14,"Q",0,"Water")</f>
+        <v>971.76621871046211</v>
       </c>
       <c r="E14">
-        <f>[2]!Props("D","T",B14,"Q",1,"Water")</f>
-        <v>0.2936721347427359</v>
+        <f>[1]!Props("D","T",B14,"Q",1,"Water")</f>
+        <v>0.29367213474305104</v>
       </c>
       <c r="F14">
-        <f>[2]!Props("H","T",B14,"Q",0,"Water")</f>
-        <v>335.01235325254447</v>
+        <f>[1]!Props("H","T",B14,"Q",0,"Water")</f>
+        <v>335.01235325239014</v>
       </c>
       <c r="G14">
-        <f>[2]!Props("H","T",B14,"Q",1,"Water")</f>
-        <v>2643.0158813452254</v>
+        <f>[1]!Props("H","T",B14,"Q",1,"Water")</f>
+        <v>2643.0158813452158</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1721,24 +1768,24 @@
         <v>363.15</v>
       </c>
       <c r="C15">
-        <f>[2]!Props("P","T",B15,"Q",0,"Water")</f>
-        <v>70.181765814537528</v>
+        <f>[1]!Props("P","T",B15,"Q",0,"Water")</f>
+        <v>70.181765815372145</v>
       </c>
       <c r="D15">
-        <f>[2]!Props("D","T",B15,"Q",0,"Water")</f>
-        <v>965.29532855043715</v>
+        <f>[1]!Props("D","T",B15,"Q",0,"Water")</f>
+        <v>965.29532855039849</v>
       </c>
       <c r="E15">
-        <f>[2]!Props("D","T",B15,"Q",1,"Water")</f>
-        <v>0.42389794463171637</v>
+        <f>[1]!Props("D","T",B15,"Q",1,"Water")</f>
+        <v>0.42389794463205877</v>
       </c>
       <c r="F15">
-        <f>[2]!Props("H","T",B15,"Q",0,"Water")</f>
-        <v>377.03938647776687</v>
+        <f>[1]!Props("H","T",B15,"Q",0,"Water")</f>
+        <v>377.03938647762016</v>
       </c>
       <c r="G15">
-        <f>[2]!Props("H","T",B15,"Q",1,"Water")</f>
-        <v>2659.5300141957478</v>
+        <f>[1]!Props("H","T",B15,"Q",1,"Water")</f>
+        <v>2659.5300141957387</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1750,24 +1797,24 @@
         <v>373.15</v>
       </c>
       <c r="C16">
-        <f>[2]!Props("P","T",B16,"Q",0,"Water")</f>
-        <v>101.41799666002106</v>
+        <f>[1]!Props("P","T",B16,"Q",0,"Water")</f>
+        <v>101.41799665916226</v>
       </c>
       <c r="D16">
-        <f>[2]!Props("D","T",B16,"Q",0,"Water")</f>
-        <v>958.34905160486005</v>
+        <f>[1]!Props("D","T",B16,"Q",0,"Water")</f>
+        <v>958.34905160482685</v>
       </c>
       <c r="E16">
-        <f>[2]!Props("D","T",B16,"Q",1,"Water")</f>
-        <v>0.5981697919259753</v>
+        <f>[1]!Props("D","T",B16,"Q",1,"Water")</f>
+        <v>0.59816979192611197</v>
       </c>
       <c r="F16">
-        <f>[2]!Props("H","T",B16,"Q",0,"Water")</f>
-        <v>419.16616289289658</v>
+        <f>[1]!Props("H","T",B16,"Q",0,"Water")</f>
+        <v>419.16616289276845</v>
       </c>
       <c r="G16">
-        <f>[2]!Props("H","T",B16,"Q",1,"Water")</f>
-        <v>2675.5698844194635</v>
+        <f>[1]!Props("H","T",B16,"Q",1,"Water")</f>
+        <v>2675.5698844194603</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1779,24 +1826,24 @@
         <v>383.15</v>
       </c>
       <c r="C17">
-        <f>[2]!Props("P","T",B17,"Q",0,"Water")</f>
-        <v>143.37871294940228</v>
+        <f>[1]!Props("P","T",B17,"Q",0,"Water")</f>
+        <v>143.37871294902544</v>
       </c>
       <c r="D17">
-        <f>[2]!Props("D","T",B17,"Q",0,"Water")</f>
-        <v>950.9480035889643</v>
+        <f>[1]!Props("D","T",B17,"Q",0,"Water")</f>
+        <v>950.94800358893906</v>
       </c>
       <c r="E17">
-        <f>[2]!Props("D","T",B17,"Q",1,"Water")</f>
-        <v>0.82692959572358737</v>
+        <f>[1]!Props("D","T",B17,"Q",1,"Water")</f>
+        <v>0.8269295957235332</v>
       </c>
       <c r="F17">
-        <f>[2]!Props("H","T",B17,"Q",0,"Water")</f>
-        <v>461.4151895343303</v>
+        <f>[1]!Props("H","T",B17,"Q",0,"Water")</f>
+        <v>461.41518953422172</v>
       </c>
       <c r="G17">
-        <f>[2]!Props("H","T",B17,"Q",1,"Water")</f>
-        <v>2691.0613426859572</v>
+        <f>[1]!Props("H","T",B17,"Q",1,"Water")</f>
+        <v>2691.0613426859577</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1808,24 +1855,24 @@
         <v>393.15</v>
       </c>
       <c r="C18">
-        <f>[2]!Props("P","T",B18,"Q",0,"Water")</f>
-        <v>198.67442047934145</v>
+        <f>[1]!Props("P","T",B18,"Q",0,"Water")</f>
+        <v>198.6744204783304</v>
       </c>
       <c r="D18">
-        <f>[2]!Props("D","T",B18,"Q",0,"Water")</f>
-        <v>943.106617430254</v>
+        <f>[1]!Props("D","T",B18,"Q",0,"Water")</f>
+        <v>943.10661743023138</v>
       </c>
       <c r="E18">
-        <f>[2]!Props("D","T",B18,"Q",1,"Water")</f>
-        <v>1.1220671917645244</v>
+        <f>[1]!Props("D","T",B18,"Q",1,"Water")</f>
+        <v>1.1220671917644258</v>
       </c>
       <c r="F18">
-        <f>[2]!Props("H","T",B18,"Q",0,"Water")</f>
-        <v>503.81169242147121</v>
+        <f>[1]!Props("H","T",B18,"Q",0,"Water")</f>
+        <v>503.81169242137508</v>
       </c>
       <c r="G18">
-        <f>[2]!Props("H","T",B18,"Q",1,"Water")</f>
-        <v>2705.9257657931835</v>
+        <f>[1]!Props("H","T",B18,"Q",1,"Water")</f>
+        <v>2705.9257657931848</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1837,24 +1884,24 @@
         <v>403.15</v>
       </c>
       <c r="C19">
-        <f>[2]!Props("P","T",B19,"Q",0,"Water")</f>
-        <v>270.27997678530858</v>
+        <f>[1]!Props("P","T",B19,"Q",0,"Water")</f>
+        <v>270.27997678512435</v>
       </c>
       <c r="D19">
-        <f>[2]!Props("D","T",B19,"Q",0,"Water")</f>
-        <v>934.83398660707985</v>
+        <f>[1]!Props("D","T",B19,"Q",0,"Water")</f>
+        <v>934.83398660706291</v>
       </c>
       <c r="E19">
-        <f>[2]!Props("D","T",B19,"Q",1,"Water")</f>
-        <v>1.4969959714828884</v>
+        <f>[1]!Props("D","T",B19,"Q",1,"Water")</f>
+        <v>1.4969959714827776</v>
       </c>
       <c r="F19">
-        <f>[2]!Props("H","T",B19,"Q",0,"Water")</f>
-        <v>546.38362438115269</v>
+        <f>[1]!Props("H","T",B19,"Q",0,"Water")</f>
+        <v>546.38362438106753</v>
       </c>
       <c r="G19">
-        <f>[2]!Props("H","T",B19,"Q",1,"Water")</f>
-        <v>2720.0811051450501</v>
+        <f>[1]!Props("H","T",B19,"Q",1,"Water")</f>
+        <v>2720.0811051450514</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1866,24 +1913,24 @@
         <v>413.15</v>
       </c>
       <c r="C20">
-        <f>[2]!Props("P","T",B20,"Q",0,"Water")</f>
-        <v>361.53909939988046</v>
+        <f>[1]!Props("P","T",B20,"Q",0,"Water")</f>
+        <v>361.53909939990245</v>
       </c>
       <c r="D20">
-        <f>[2]!Props("D","T",B20,"Q",0,"Water")</f>
-        <v>926.13441329112413</v>
+        <f>[1]!Props("D","T",B20,"Q",0,"Water")</f>
+        <v>926.13441329111174</v>
       </c>
       <c r="E20">
-        <f>[2]!Props("D","T",B20,"Q",1,"Water")</f>
-        <v>1.9667450045125305</v>
+        <f>[1]!Props("D","T",B20,"Q",1,"Water")</f>
+        <v>1.966745004512499</v>
       </c>
       <c r="F20">
-        <f>[2]!Props("H","T",B20,"Q",0,"Water")</f>
-        <v>589.16169048823679</v>
+        <f>[1]!Props("H","T",B20,"Q",0,"Water")</f>
+        <v>589.16169048816187</v>
       </c>
       <c r="G20">
-        <f>[2]!Props("H","T",B20,"Q",1,"Water")</f>
-        <v>2733.4429731737555</v>
+        <f>[1]!Props("H","T",B20,"Q",1,"Water")</f>
+        <v>2733.4429731737559</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1895,24 +1942,24 @@
         <v>423.15</v>
       </c>
       <c r="C21">
-        <f>[2]!Props("P","T",B21,"Q",0,"Water")</f>
-        <v>476.16453797031113</v>
+        <f>[1]!Props("P","T",B21,"Q",0,"Water")</f>
+        <v>476.16453796936935</v>
       </c>
       <c r="D21">
-        <f>[2]!Props("D","T",B21,"Q",0,"Water")</f>
-        <v>917.00773926892555</v>
+        <f>[1]!Props("D","T",B21,"Q",0,"Water")</f>
+        <v>917.00773926891372</v>
       </c>
       <c r="E21">
-        <f>[2]!Props("D","T",B21,"Q",1,"Water")</f>
-        <v>2.5480771470961141</v>
+        <f>[1]!Props("D","T",B21,"Q",1,"Water")</f>
+        <v>2.5480771470965995</v>
       </c>
       <c r="F21">
-        <f>[2]!Props("H","T",B21,"Q",0,"Water")</f>
-        <v>632.17944178056644</v>
+        <f>[1]!Props("H","T",B21,"Q",0,"Water")</f>
+        <v>632.17944178050175</v>
       </c>
       <c r="G21">
-        <f>[2]!Props("H","T",B21,"Q",1,"Water")</f>
-        <v>2745.9254514300796</v>
+        <f>[1]!Props("H","T",B21,"Q",1,"Water")</f>
+        <v>2745.9254514300715</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1924,24 +1971,24 @@
         <v>433.15</v>
       </c>
       <c r="C22">
-        <f>[2]!Props("P","T",B22,"Q",0,"Water")</f>
-        <v>618.23462142577796</v>
+        <f>[1]!Props("P","T",B22,"Q",0,"Water")</f>
+        <v>618.23462142627261</v>
       </c>
       <c r="D22">
-        <f>[2]!Props("D","T",B22,"Q",0,"Water")</f>
-        <v>907.44950563407349</v>
+        <f>[1]!Props("D","T",B22,"Q",0,"Water")</f>
+        <v>907.44950563406553</v>
       </c>
       <c r="E22">
-        <f>[2]!Props("D","T",B22,"Q",1,"Water")</f>
-        <v>3.2596441977608386</v>
+        <f>[1]!Props("D","T",B22,"Q",1,"Water")</f>
+        <v>3.2596441977622423</v>
       </c>
       <c r="F22">
-        <f>[2]!Props("H","T",B22,"Q",0,"Water")</f>
-        <v>675.47346558322408</v>
+        <f>[1]!Props("H","T",B22,"Q",0,"Water")</f>
+        <v>675.47346558316849</v>
       </c>
       <c r="G22">
-        <f>[2]!Props("H","T",B22,"Q",1,"Water")</f>
-        <v>2757.4413489921203</v>
+        <f>[1]!Props("H","T",B22,"Q",1,"Water")</f>
+        <v>2757.441348992098</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1953,24 +2000,24 @@
         <v>443.15</v>
       </c>
       <c r="C23">
-        <f>[2]!Props("P","T",B23,"Q",0,"Water")</f>
-        <v>792.18700698190401</v>
+        <f>[1]!Props("P","T",B23,"Q",0,"Water")</f>
+        <v>792.18700698253531</v>
       </c>
       <c r="D23">
-        <f>[2]!Props("D","T",B23,"Q",0,"Water")</f>
-        <v>897.45096587597288</v>
+        <f>[1]!Props("D","T",B23,"Q",0,"Water")</f>
+        <v>897.45096587596697</v>
       </c>
       <c r="E23">
-        <f>[2]!Props("D","T",B23,"Q",1,"Water")</f>
-        <v>4.1221925343361514</v>
+        <f>[1]!Props("D","T",B23,"Q",1,"Water")</f>
+        <v>4.1221925343383052</v>
       </c>
       <c r="F23">
-        <f>[2]!Props("H","T",B23,"Q",0,"Water")</f>
-        <v>719.08369096295746</v>
+        <f>[1]!Props("H","T",B23,"Q",0,"Water")</f>
+        <v>719.08369096290494</v>
       </c>
       <c r="G23">
-        <f>[2]!Props("H","T",B23,"Q",1,"Water")</f>
-        <v>2767.901762261462</v>
+        <f>[1]!Props("H","T",B23,"Q",1,"Water")</f>
+        <v>2767.9017622614292</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1982,24 +2029,24 @@
         <v>453.15</v>
       </c>
       <c r="C24">
-        <f>[2]!Props("P","T",B24,"Q",0,"Water")</f>
-        <v>1002.8105360782905</v>
+        <f>[1]!Props("P","T",B24,"Q",0,"Water")</f>
+        <v>1002.8105360782382</v>
       </c>
       <c r="D24">
-        <f>[2]!Props("D","T",B24,"Q",0,"Water")</f>
-        <v>886.99896128082025</v>
+        <f>[1]!Props("D","T",B24,"Q",0,"Water")</f>
+        <v>886.99896128081559</v>
       </c>
       <c r="E24">
-        <f>[2]!Props("D","T",B24,"Q",1,"Water")</f>
-        <v>5.1588361289185185</v>
+        <f>[1]!Props("D","T",B24,"Q",1,"Water")</f>
+        <v>5.1588361289205622</v>
       </c>
       <c r="F24">
-        <f>[2]!Props("H","T",B24,"Q",0,"Water")</f>
-        <v>763.05382639583047</v>
+        <f>[1]!Props("H","T",B24,"Q",0,"Water")</f>
+        <v>763.05382639578045</v>
       </c>
       <c r="G24">
-        <f>[2]!Props("H","T",B24,"Q",1,"Water")</f>
-        <v>2777.2149260216215</v>
+        <f>[1]!Props("H","T",B24,"Q",1,"Water")</f>
+        <v>2777.2149260215924</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2011,24 +2058,24 @@
         <v>463.15</v>
       </c>
       <c r="C25">
-        <f>[2]!Props("P","T",B25,"Q",0,"Water")</f>
-        <v>1255.2361551605081</v>
+        <f>[1]!Props("P","T",B25,"Q",0,"Water")</f>
+        <v>1255.2361551608849</v>
       </c>
       <c r="D25">
-        <f>[2]!Props("D","T",B25,"Q",0,"Water")</f>
-        <v>876.07565429885642</v>
+        <f>[1]!Props("D","T",B25,"Q",0,"Water")</f>
+        <v>876.07565429885472</v>
       </c>
       <c r="E25">
-        <f>[2]!Props("D","T",B25,"Q",1,"Water")</f>
-        <v>6.3954187812079395</v>
+        <f>[1]!Props("D","T",B25,"Q",1,"Water")</f>
+        <v>6.3954187812090098</v>
       </c>
       <c r="F25">
-        <f>[2]!Props("H","T",B25,"Q",0,"Water")</f>
-        <v>807.43195145025493</v>
+        <f>[1]!Props("H","T",B25,"Q",0,"Water")</f>
+        <v>807.43195145020456</v>
       </c>
       <c r="G25">
-        <f>[2]!Props("H","T",B25,"Q",1,"Water")</f>
-        <v>2785.2844447620487</v>
+        <f>[1]!Props("H","T",B25,"Q",1,"Water")</f>
+        <v>2785.2844447620337</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2040,24 +2087,24 @@
         <v>473.15</v>
       </c>
       <c r="C26">
-        <f>[2]!Props("P","T",B26,"Q",0,"Water")</f>
-        <v>1554.9279004667762</v>
+        <f>[1]!Props("P","T",B26,"Q",0,"Water")</f>
+        <v>1554.9279004671425</v>
       </c>
       <c r="D26">
-        <f>[2]!Props("D","T",B26,"Q",0,"Water")</f>
-        <v>864.65810228712542</v>
+        <f>[1]!Props("D","T",B26,"Q",0,"Water")</f>
+        <v>864.65810228712428</v>
       </c>
       <c r="E26">
-        <f>[2]!Props("D","T",B26,"Q",1,"Water")</f>
-        <v>7.860994516784042</v>
+        <f>[1]!Props("D","T",B26,"Q",1,"Water")</f>
+        <v>7.860994516784233</v>
       </c>
       <c r="F26">
-        <f>[2]!Props("H","T",B26,"Q",0,"Water")</f>
-        <v>852.27129446018387</v>
+        <f>[1]!Props("H","T",B26,"Q",0,"Water")</f>
+        <v>852.27129446014476</v>
       </c>
       <c r="G26">
-        <f>[2]!Props("H","T",B26,"Q",1,"Water")</f>
-        <v>2792.0070226267294</v>
+        <f>[1]!Props("H","T",B26,"Q",1,"Water")</f>
+        <v>2792.0070226267262</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2069,24 +2116,24 @@
         <v>483.15</v>
       </c>
       <c r="C27">
-        <f>[2]!Props("P","T",B27,"Q",0,"Water")</f>
-        <v>1907.6749935324397</v>
+        <f>[1]!Props("P","T",B27,"Q",0,"Water")</f>
+        <v>1907.6749935317039</v>
       </c>
       <c r="D27">
-        <f>[2]!Props("D","T",B27,"Q",0,"Water")</f>
-        <v>852.71763851005721</v>
+        <f>[1]!Props("D","T",B27,"Q",0,"Water")</f>
+        <v>852.71763851005528</v>
       </c>
       <c r="E27">
-        <f>[2]!Props("D","T",B27,"Q",1,"Water")</f>
-        <v>9.5884655414267677</v>
+        <f>[1]!Props("D","T",B27,"Q",1,"Water")</f>
+        <v>9.5884655414265385</v>
       </c>
       <c r="F27">
-        <f>[2]!Props("H","T",B27,"Q",0,"Water")</f>
-        <v>897.63124444416621</v>
+        <f>[1]!Props("H","T",B27,"Q",0,"Water")</f>
+        <v>897.63124444412767</v>
       </c>
       <c r="G27">
-        <f>[2]!Props("H","T",B27,"Q",1,"Water")</f>
-        <v>2797.2697683428019</v>
+        <f>[1]!Props("H","T",B27,"Q",1,"Water")</f>
+        <v>2797.2697683428046</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2098,24 +2145,24 @@
         <v>493.15</v>
       </c>
       <c r="C28">
-        <f>[2]!Props("P","T",B28,"Q",0,"Water")</f>
-        <v>2319.5861701998538</v>
+        <f>[1]!Props("P","T",B28,"Q",0,"Water")</f>
+        <v>2319.5861702587372</v>
       </c>
       <c r="D28">
-        <f>[2]!Props("D","T",B28,"Q",0,"Water")</f>
-        <v>840.21900675000336</v>
+        <f>[1]!Props("D","T",B28,"Q",0,"Water")</f>
+        <v>840.21900675010761</v>
       </c>
       <c r="E28">
-        <f>[2]!Props("D","T",B28,"Q",1,"Water")</f>
-        <v>11.615432874295058</v>
+        <f>[1]!Props("D","T",B28,"Q",1,"Water")</f>
+        <v>11.615432874294592</v>
       </c>
       <c r="F28">
-        <f>[2]!Props("H","T",B28,"Q",0,"Water")</f>
-        <v>943.5786700422118</v>
+        <f>[1]!Props("H","T",B28,"Q",0,"Water")</f>
+        <v>943.57867004221146</v>
       </c>
       <c r="G28">
-        <f>[2]!Props("H","T",B28,"Q",1,"Water")</f>
-        <v>2800.9470527725616</v>
+        <f>[1]!Props("H","T",B28,"Q",1,"Water")</f>
+        <v>2800.9470527725671</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2127,24 +2174,24 @@
         <v>503.15</v>
       </c>
       <c r="C29">
-        <f>[2]!Props("P","T",B29,"Q",0,"Water")</f>
-        <v>2797.0874969297211</v>
+        <f>[1]!Props("P","T",B29,"Q",0,"Water")</f>
+        <v>2797.0874969298998</v>
       </c>
       <c r="D29">
-        <f>[2]!Props("D","T",B29,"Q",0,"Water")</f>
-        <v>827.11916655179948</v>
+        <f>[1]!Props("D","T",B29,"Q",0,"Water")</f>
+        <v>827.11916655180175</v>
       </c>
       <c r="E29">
-        <f>[2]!Props("D","T",B29,"Q",1,"Water")</f>
-        <v>13.98533895750848</v>
+        <f>[1]!Props("D","T",B29,"Q",1,"Water")</f>
+        <v>13.985338957508098</v>
       </c>
       <c r="F29">
-        <f>[2]!Props("H","T",B29,"Q",0,"Water")</f>
-        <v>990.18965507747453</v>
+        <f>[1]!Props("H","T",B29,"Q",0,"Water")</f>
+        <v>990.1896550774411</v>
       </c>
       <c r="G29">
-        <f>[2]!Props("H","T",B29,"Q",1,"Water")</f>
-        <v>2802.8967584010438</v>
+        <f>[1]!Props("H","T",B29,"Q",1,"Water")</f>
+        <v>2802.8967584010479</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2156,24 +2203,24 @@
         <v>513.15</v>
       </c>
       <c r="C30">
-        <f>[2]!Props("P","T",B30,"Q",0,"Water")</f>
-        <v>3346.9251442691252</v>
+        <f>[1]!Props("P","T",B30,"Q",0,"Water")</f>
+        <v>3346.9251442694003</v>
       </c>
       <c r="D30">
-        <f>[2]!Props("D","T",B30,"Q",0,"Water")</f>
-        <v>813.36564216909892</v>
+        <f>[1]!Props("D","T",B30,"Q",0,"Water")</f>
+        <v>813.36564216910097</v>
       </c>
       <c r="E30">
-        <f>[2]!Props("D","T",B30,"Q",1,"Water")</f>
-        <v>16.749019301603251</v>
+        <f>[1]!Props("D","T",B30,"Q",1,"Water")</f>
+        <v>16.749019301602761</v>
       </c>
       <c r="F30">
-        <f>[2]!Props("H","T",B30,"Q",0,"Water")</f>
-        <v>1037.5518165790263</v>
+        <f>[1]!Props("H","T",B30,"Q",0,"Water")</f>
+        <v>1037.551816578999</v>
       </c>
       <c r="G30">
-        <f>[2]!Props("H","T",B30,"Q",1,"Water")</f>
-        <v>2802.9556046252342</v>
+        <f>[1]!Props("H","T",B30,"Q",1,"Water")</f>
+        <v>2802.9556046252392</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2185,24 +2232,24 @@
         <v>523.15</v>
       </c>
       <c r="C31">
-        <f>[2]!Props("P","T",B31,"Q",0,"Water")</f>
-        <v>3976.1749306524707</v>
+        <f>[1]!Props("P","T",B31,"Q",0,"Water")</f>
+        <v>3976.1749306524598</v>
       </c>
       <c r="D31">
-        <f>[2]!Props("D","T",B31,"Q",0,"Water")</f>
-        <v>798.89422022042186</v>
+        <f>[1]!Props("D","T",B31,"Q",0,"Water")</f>
+        <v>798.89422022042652</v>
       </c>
       <c r="E31">
-        <f>[2]!Props("D","T",B31,"Q",1,"Water")</f>
-        <v>19.966840438464651</v>
+        <f>[1]!Props("D","T",B31,"Q",1,"Water")</f>
+        <v>19.966840438464143</v>
       </c>
       <c r="F31">
-        <f>[2]!Props("H","T",B31,"Q",0,"Water")</f>
-        <v>1085.7674588110503</v>
+        <f>[1]!Props("H","T",B31,"Q",0,"Water")</f>
+        <v>1085.7674588110201</v>
       </c>
       <c r="G31">
-        <f>[2]!Props("H","T",B31,"Q",1,"Water")</f>
-        <v>2800.9330729758321</v>
+        <f>[1]!Props("H","T",B31,"Q",1,"Water")</f>
+        <v>2800.9330729758371</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2214,24 +2261,24 @@
         <v>533.15</v>
       </c>
       <c r="C32">
-        <f>[2]!Props("P","T",B32,"Q",0,"Water")</f>
-        <v>4692.260992299709</v>
+        <f>[1]!Props("P","T",B32,"Q",0,"Water")</f>
+        <v>4692.2609922994561</v>
       </c>
       <c r="D32">
-        <f>[2]!Props("D","T",B32,"Q",0,"Water")</f>
-        <v>783.62569286973383</v>
+        <f>[1]!Props("D","T",B32,"Q",0,"Water")</f>
+        <v>783.62569286973826</v>
       </c>
       <c r="E32">
-        <f>[2]!Props("D","T",B32,"Q",1,"Water")</f>
-        <v>23.711700367712265</v>
+        <f>[1]!Props("D","T",B32,"Q",1,"Water")</f>
+        <v>23.711700367711778</v>
       </c>
       <c r="F32">
-        <f>[2]!Props("H","T",B32,"Q",0,"Water")</f>
-        <v>1134.9579569891296</v>
+        <f>[1]!Props("H","T",B32,"Q",0,"Water")</f>
+        <v>1134.9579569891007</v>
       </c>
       <c r="G32">
-        <f>[2]!Props("H","T",B32,"Q",1,"Water")</f>
-        <v>2796.6032203853524</v>
+        <f>[1]!Props("H","T",B32,"Q",1,"Water")</f>
+        <v>2796.6032203853574</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2243,24 +2290,24 @@
         <v>543.15</v>
       </c>
       <c r="C33">
-        <f>[2]!Props("P","T",B33,"Q",0,"Water")</f>
-        <v>5502.986783014605</v>
+        <f>[1]!Props("P","T",B33,"Q",0,"Water")</f>
+        <v>5502.9867830146577</v>
       </c>
       <c r="D33">
-        <f>[2]!Props("D","T",B33,"Q",0,"Water")</f>
-        <v>767.46116679898125</v>
+        <f>[1]!Props("D","T",B33,"Q",0,"Water")</f>
+        <v>767.46116679898569</v>
       </c>
       <c r="E33">
-        <f>[2]!Props("D","T",B33,"Q",1,"Water")</f>
-        <v>28.07333562442464</v>
+        <f>[1]!Props("D","T",B33,"Q",1,"Water")</f>
+        <v>28.073335624423731</v>
       </c>
       <c r="F33">
-        <f>[2]!Props("H","T",B33,"Q",0,"Water")</f>
-        <v>1185.2699943566126</v>
+        <f>[1]!Props("H","T",B33,"Q",0,"Water")</f>
+        <v>1185.2699943565901</v>
       </c>
       <c r="G33">
-        <f>[2]!Props("H","T",B33,"Q",1,"Water")</f>
-        <v>2789.6932193000084</v>
+        <f>[1]!Props("H","T",B33,"Q",1,"Water")</f>
+        <v>2789.6932193000157</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2272,24 +2319,24 @@
         <v>553.15</v>
       </c>
       <c r="C34">
-        <f>[2]!Props("P","T",B34,"Q",0,"Water")</f>
-        <v>6416.582909532026</v>
+        <f>[1]!Props("P","T",B34,"Q",0,"Water")</f>
+        <v>6416.5829095316267</v>
       </c>
       <c r="D34">
-        <f>[2]!Props("D","T",B34,"Q",0,"Water")</f>
-        <v>750.27516129988351</v>
+        <f>[1]!Props("D","T",B34,"Q",0,"Water")</f>
+        <v>750.27516129988749</v>
       </c>
       <c r="E34">
-        <f>[2]!Props("D","T",B34,"Q",1,"Water")</f>
-        <v>33.164674054045683</v>
+        <f>[1]!Props("D","T",B34,"Q",1,"Water")</f>
+        <v>33.164674054045257</v>
       </c>
       <c r="F34">
-        <f>[2]!Props("H","T",B34,"Q",0,"Water")</f>
-        <v>1236.8846659592693</v>
+        <f>[1]!Props("H","T",B34,"Q",0,"Water")</f>
+        <v>1236.8846659592452</v>
       </c>
       <c r="G34">
-        <f>[2]!Props("H","T",B34,"Q",1,"Water")</f>
-        <v>2779.8667305294553</v>
+        <f>[1]!Props("H","T",B34,"Q",1,"Water")</f>
+        <v>2779.8667305294593</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2301,24 +2348,24 @@
         <v>563.15</v>
       </c>
       <c r="C35">
-        <f>[2]!Props("P","T",B35,"Q",0,"Water")</f>
-        <v>7441.7783444212137</v>
+        <f>[1]!Props("P","T",B35,"Q",0,"Water")</f>
+        <v>7441.7783444209954</v>
       </c>
       <c r="D35">
-        <f>[2]!Props("D","T",B35,"Q",0,"Water")</f>
-        <v>731.9051996436865</v>
+        <f>[1]!Props("D","T",B35,"Q",0,"Water")</f>
+        <v>731.90519964369241</v>
       </c>
       <c r="E35">
-        <f>[2]!Props("D","T",B35,"Q",1,"Water")</f>
-        <v>39.131512960158695</v>
+        <f>[1]!Props("D","T",B35,"Q",1,"Water")</f>
+        <v>39.131512960157593</v>
       </c>
       <c r="F35">
-        <f>[2]!Props("H","T",B35,"Q",0,"Water")</f>
-        <v>1290.0311497479681</v>
+        <f>[1]!Props("H","T",B35,"Q",0,"Water")</f>
+        <v>1290.0311497479454</v>
       </c>
       <c r="G35">
-        <f>[2]!Props("H","T",B35,"Q",1,"Water")</f>
-        <v>2766.6990506391335</v>
+        <f>[1]!Props("H","T",B35,"Q",1,"Water")</f>
+        <v>2766.6990506391412</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2330,24 +2377,24 @@
         <v>573.15</v>
       </c>
       <c r="C36">
-        <f>[2]!Props("P","T",B36,"Q",0,"Water")</f>
-        <v>8587.9049408353676</v>
+        <f>[1]!Props("P","T",B36,"Q",0,"Water")</f>
+        <v>8587.9049408353076</v>
       </c>
       <c r="D36">
-        <f>[2]!Props("D","T",B36,"Q",0,"Water")</f>
-        <v>712.13563881961431</v>
+        <f>[1]!Props("D","T",B36,"Q",0,"Water")</f>
+        <v>712.13563881962102</v>
       </c>
       <c r="E36">
-        <f>[2]!Props("D","T",B36,"Q",1,"Water")</f>
-        <v>46.167849523794111</v>
+        <f>[1]!Props("D","T",B36,"Q",1,"Water")</f>
+        <v>46.167849523793365</v>
       </c>
       <c r="F36">
-        <f>[2]!Props("H","T",B36,"Q",0,"Water")</f>
-        <v>1345.0079264161157</v>
+        <f>[1]!Props("H","T",B36,"Q",0,"Water")</f>
+        <v>1345.0079264160959</v>
       </c>
       <c r="G36">
-        <f>[2]!Props("H","T",B36,"Q",1,"Water")</f>
-        <v>2749.6387614002501</v>
+        <f>[1]!Props("H","T",B36,"Q",1,"Water")</f>
+        <v>2749.6387614002556</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2359,24 +2406,24 @@
         <v>583.15</v>
       </c>
       <c r="C37">
-        <f>[2]!Props("P","T",B37,"Q",0,"Water")</f>
-        <v>9865.0512111820826</v>
+        <f>[1]!Props("P","T",B37,"Q",0,"Water")</f>
+        <v>9865.0512111816915</v>
       </c>
       <c r="D37">
-        <f>[2]!Props("D","T",B37,"Q",0,"Water")</f>
-        <v>690.67154560984363</v>
+        <f>[1]!Props("D","T",B37,"Q",0,"Water")</f>
+        <v>690.67154560985284</v>
       </c>
       <c r="E37">
-        <f>[2]!Props("D","T",B37,"Q",1,"Water")</f>
-        <v>54.541361541638153</v>
+        <f>[1]!Props("D","T",B37,"Q",1,"Water")</f>
+        <v>54.541361541637151</v>
       </c>
       <c r="F37">
-        <f>[2]!Props("H","T",B37,"Q",0,"Water")</f>
-        <v>1402.2171260009688</v>
+        <f>[1]!Props("H","T",B37,"Q",0,"Water")</f>
+        <v>1402.2171260009461</v>
       </c>
       <c r="G37">
-        <f>[2]!Props("H","T",B37,"Q",1,"Water")</f>
-        <v>2727.9458789653868</v>
+        <f>[1]!Props("H","T",B37,"Q",1,"Water")</f>
+        <v>2727.9458789653931</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2388,24 +2435,24 @@
         <v>593.15</v>
       </c>
       <c r="C38">
-        <f>[2]!Props("P","T",B38,"Q",0,"Water")</f>
-        <v>11284.292927464725</v>
+        <f>[1]!Props("P","T",B38,"Q",0,"Water")</f>
+        <v>11284.292927464572</v>
       </c>
       <c r="D38">
-        <f>[2]!Props("D","T",B38,"Q",0,"Water")</f>
-        <v>667.09384803259525</v>
+        <f>[1]!Props("D","T",B38,"Q",0,"Water")</f>
+        <v>667.09384803260423</v>
       </c>
       <c r="E38">
-        <f>[2]!Props("D","T",B38,"Q",1,"Water")</f>
-        <v>64.638432419886186</v>
+        <f>[1]!Props("D","T",B38,"Q",1,"Water")</f>
+        <v>64.638432419885376</v>
       </c>
       <c r="F38">
-        <f>[2]!Props("H","T",B38,"Q",0,"Water")</f>
-        <v>1462.2236463970917</v>
+        <f>[1]!Props("H","T",B38,"Q",0,"Water")</f>
+        <v>1462.2236463970723</v>
       </c>
       <c r="G38">
-        <f>[2]!Props("H","T",B38,"Q",1,"Water")</f>
-        <v>2700.5857692409354</v>
+        <f>[1]!Props("H","T",B38,"Q",1,"Water")</f>
+        <v>2700.5857692409404</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2417,24 +2464,24 @@
         <v>603.15</v>
       </c>
       <c r="C39">
-        <f>[2]!Props("P","T",B39,"Q",0,"Water")</f>
-        <v>12858.051600018429</v>
+        <f>[1]!Props("P","T",B39,"Q",0,"Water")</f>
+        <v>12858.051600204713</v>
       </c>
       <c r="D39">
-        <f>[2]!Props("D","T",B39,"Q",0,"Water")</f>
-        <v>640.7732152647435</v>
+        <f>[1]!Props("D","T",B39,"Q",0,"Water")</f>
+        <v>640.77321526640685</v>
       </c>
       <c r="E39">
-        <f>[2]!Props("D","T",B39,"Q",1,"Water")</f>
-        <v>77.05042598731238</v>
+        <f>[1]!Props("D","T",B39,"Q",1,"Water")</f>
+        <v>77.050425987311172</v>
       </c>
       <c r="F39">
-        <f>[2]!Props("H","T",B39,"Q",0,"Water")</f>
-        <v>1525.8683270564179</v>
+        <f>[1]!Props("H","T",B39,"Q",0,"Water")</f>
+        <v>1525.8683270550459</v>
       </c>
       <c r="G39">
-        <f>[2]!Props("H","T",B39,"Q",1,"Water")</f>
-        <v>2666.0311405571751</v>
+        <f>[1]!Props("H","T",B39,"Q",1,"Water")</f>
+        <v>2666.031140557182</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2446,24 +2493,24 @@
         <v>613.15</v>
       </c>
       <c r="C40">
-        <f>[2]!Props("P","T",B40,"Q",0,"Water")</f>
-        <v>14600.677371948063</v>
+        <f>[1]!Props("P","T",B40,"Q",0,"Water")</f>
+        <v>14600.677372002207</v>
       </c>
       <c r="D40">
-        <f>[2]!Props("D","T",B40,"Q",0,"Water")</f>
-        <v>610.66759832473281</v>
+        <f>[1]!Props("D","T",B40,"Q",0,"Water")</f>
+        <v>610.66759832541493</v>
       </c>
       <c r="E40">
-        <f>[2]!Props("D","T",B40,"Q",1,"Water")</f>
-        <v>92.758782507416598</v>
+        <f>[1]!Props("D","T",B40,"Q",1,"Water")</f>
+        <v>92.758782507415674</v>
       </c>
       <c r="F40">
-        <f>[2]!Props("H","T",B40,"Q",0,"Water")</f>
-        <v>1594.5289922369011</v>
+        <f>[1]!Props("H","T",B40,"Q",0,"Water")</f>
+        <v>1594.5289922362745</v>
       </c>
       <c r="G40">
-        <f>[2]!Props("H","T",B40,"Q",1,"Water")</f>
-        <v>2621.8455755251834</v>
+        <f>[1]!Props("H","T",B40,"Q",1,"Water")</f>
+        <v>2621.8455755251885</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2475,24 +2522,24 @@
         <v>623.15</v>
       </c>
       <c r="C41">
-        <f>[2]!Props("P","T",B41,"Q",0,"Water")</f>
-        <v>16529.415139004064</v>
+        <f>[1]!Props("P","T",B41,"Q",0,"Water")</f>
+        <v>16529.415139051285</v>
       </c>
       <c r="D41">
-        <f>[2]!Props("D","T",B41,"Q",0,"Water")</f>
-        <v>574.70651653672451</v>
+        <f>[1]!Props("D","T",B41,"Q",0,"Water")</f>
+        <v>574.70651653765685</v>
       </c>
       <c r="E41">
-        <f>[2]!Props("D","T",B41,"Q",1,"Water")</f>
-        <v>113.60561050163348</v>
+        <f>[1]!Props("D","T",B41,"Q",1,"Water")</f>
+        <v>113.60561050162028</v>
       </c>
       <c r="F41">
-        <f>[2]!Props("H","T",B41,"Q",0,"Water")</f>
-        <v>1670.8899067287161</v>
+        <f>[1]!Props("H","T",B41,"Q",0,"Water")</f>
+        <v>1670.8899067277875</v>
       </c>
       <c r="G41">
-        <f>[2]!Props("H","T",B41,"Q",1,"Water")</f>
-        <v>2563.6367109445368</v>
+        <f>[1]!Props("H","T",B41,"Q",1,"Water")</f>
+        <v>2563.6367109445987</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2504,24 +2551,24 @@
         <v>633.15</v>
       </c>
       <c r="C42">
-        <f>[2]!Props("P","T",B42,"Q",0,"Water")</f>
-        <v>18666.006645644644</v>
+        <f>[1]!Props("P","T",B42,"Q",0,"Water")</f>
+        <v>18666.006646276048</v>
       </c>
       <c r="D42">
-        <f>[2]!Props("D","T",B42,"Q",0,"Water")</f>
-        <v>527.59162939688963</v>
+        <f>[1]!Props("D","T",B42,"Q",0,"Water")</f>
+        <v>527.59162942231876</v>
       </c>
       <c r="E42">
-        <f>[2]!Props("D","T",B42,"Q",1,"Water")</f>
-        <v>143.89841140942264</v>
+        <f>[1]!Props("D","T",B42,"Q",1,"Water")</f>
+        <v>143.89841140848043</v>
       </c>
       <c r="F42">
-        <f>[2]!Props("H","T",B42,"Q",0,"Water")</f>
-        <v>1761.6646205625962</v>
+        <f>[1]!Props("H","T",B42,"Q",0,"Water")</f>
+        <v>1761.6646205355191</v>
       </c>
       <c r="G42">
-        <f>[2]!Props("H","T",B42,"Q",1,"Water")</f>
-        <v>2481.4924833322702</v>
+        <f>[1]!Props("H","T",B42,"Q",1,"Water")</f>
+        <v>2481.4924833359923</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2533,54 +2580,54 @@
         <v>643.15</v>
       </c>
       <c r="C43">
-        <f>[2]!Props("P","T",B43,"Q",0,"Water")</f>
-        <v>21043.56314746592</v>
+        <f>[1]!Props("P","T",B43,"Q",0,"Water")</f>
+        <v>21043.563147465924</v>
       </c>
       <c r="D43">
-        <f>[2]!Props("D","T",B43,"Q",0,"Water")</f>
-        <v>451.42564747531384</v>
+        <f>[1]!Props("D","T",B43,"Q",0,"Water")</f>
+        <v>451.42564747534033</v>
       </c>
       <c r="E43">
-        <f>[2]!Props("D","T",B43,"Q",1,"Water")</f>
-        <v>201.83931641744371</v>
+        <f>[1]!Props("D","T",B43,"Q",1,"Water")</f>
+        <v>201.83931641744931</v>
       </c>
       <c r="F43">
-        <f>[2]!Props("H","T",B43,"Q",0,"Water")</f>
-        <v>1890.6872488661784</v>
+        <f>[1]!Props("H","T",B43,"Q",0,"Water")</f>
+        <v>1890.6872488661456</v>
       </c>
       <c r="G43">
-        <f>[2]!Props("H","T",B43,"Q",1,"Water")</f>
-        <v>2334.5182916068165</v>
+        <f>[1]!Props("H","T",B43,"Q",1,"Water")</f>
+        <v>2334.5182916067993</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <f>[2]!Props1("Water","Tcrit")-0.01-273.15</f>
-        <v>373.93600000000004</v>
-      </c>
-      <c r="B44" s="2">
-        <f t="shared" ref="B44" si="1">A44+273.15</f>
-        <v>647.08600000000001</v>
-      </c>
-      <c r="C44">
-        <f>[2]!Props("P","T",B44,"Q",0,"Water")</f>
-        <v>22061.328131850038</v>
-      </c>
-      <c r="D44">
-        <f>[2]!Props("D","T",B44,"Q",0,"Water")</f>
-        <v>337.04410411346163</v>
-      </c>
-      <c r="E44">
-        <f>[2]!Props("D","T",B44,"Q",1,"Water")</f>
-        <v>306.79658492825473</v>
-      </c>
-      <c r="F44">
-        <f>[2]!Props("H","T",B44,"Q",0,"Water")</f>
-        <v>2060.0042388923648</v>
-      </c>
-      <c r="G44">
-        <f>[2]!Props("H","T",B44,"Q",1,"Water")</f>
-        <v>2110.5585219387103</v>
+      <c r="A44" t="e">
+        <f ca="1">[1]!Props1("Water","Tcrit")-0.01-273.15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B44" s="2" t="e">
+        <f t="shared" ref="B44" ca="1" si="1">A44+273.15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C44" t="e">
+        <f ca="1">[1]!Props("P","T",B44,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D44" t="e">
+        <f ca="1">[1]!Props("D","T",B44,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E44" t="e">
+        <f ca="1">[1]!Props("D","T",B44,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F44" t="e">
+        <f ca="1">[1]!Props("H","T",B44,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G44" t="e">
+        <f ca="1">[1]!Props("H","T",B44,"Q",1,"Water")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug in VBA code; see #805
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Critical temperature of R410A:</t>
   </si>
@@ -207,10 +207,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,7 +806,7 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:axId val="123193984"/>
-        <c:axId val="123753216"/>
+        <c:axId val="123720448"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="123193984"/>
@@ -837,12 +837,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123753216"/>
+        <c:crossAx val="123720448"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123753216"/>
+        <c:axId val="123720448"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1238,14 +1238,14 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.42578125" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,6 +1287,9 @@
         <f>[1]!Props1SI("R410A","Tcrit")</f>
         <v>344.49400000000003</v>
       </c>
+      <c r="D6">
+        <v>344.49400000000003</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1299,6 +1302,9 @@
         <f>[1]!Props1SI("Propane","rhocrit")</f>
         <v>220.47810000000004</v>
       </c>
+      <c r="D7">
+        <v>220.47810000000004</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1311,6 +1317,9 @@
         <f>[1]!PropsSI("Dmass","T",298.15,"P",101325,"HEOS::Nitrogen")</f>
         <v>1.1452448929366676</v>
       </c>
+      <c r="D8">
+        <v>1.1452448929366676</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1323,6 +1332,9 @@
         <f>[1]!PropsSI("T","P",101325,"Q",0,"HEOS::Water")-273.15</f>
         <v>99.97429584768804</v>
       </c>
+      <c r="D9">
+        <v>99.97429584768804</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1335,6 +1347,9 @@
         <f>[1]!PropsSI("T","P",101325,"Q",0,"REFPROP::Water")-273.15</f>
         <v>99.974295847697988</v>
       </c>
+      <c r="D10">
+        <v>99.974295847697988</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1356,6 +1371,9 @@
         <f>[1]!PropsSI("V","T",300,"P",101.325,"INCOMP::MEG[0.2]")</f>
         <v>1.38142216644215E-3</v>
       </c>
+      <c r="D12">
+        <v>1.38142216644215E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1363,7 +1381,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1375,7 +1393,7 @@
         <v>0.78090000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1383,7 +1401,7 @@
         <v>0.20949999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1391,7 +1409,7 @@
         <v>9.2999999999999992E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1399,12 +1417,18 @@
         <v>3.8999999999999999E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
       <c r="C20">
         <f>[1]!PropsSI("T","P",101325,"Q",0,"HEOS::"&amp;[1]!MixtureString(A16:A19,B16:B19))</f>
+        <v>78.650190680028572</v>
+      </c>
+      <c r="D20">
         <v>78.650190680028572</v>
       </c>
     </row>
@@ -1430,13 +1454,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Fixed order of oxygen and argon in sample file for excel
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -805,11 +805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123193984"/>
-        <c:axId val="123720448"/>
+        <c:axId val="123128448"/>
+        <c:axId val="125776640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123193984"/>
+        <c:axId val="123128448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,12 +837,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123720448"/>
+        <c:crossAx val="125776640"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123720448"/>
+        <c:axId val="125776640"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -871,7 +871,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123193984"/>
+        <c:crossAx val="123128448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>0.20949999999999999</v>
@@ -1403,7 +1403,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18">
         <v>9.2999999999999992E-3</v>
@@ -1426,10 +1426,10 @@
       </c>
       <c r="C20">
         <f>[1]!PropsSI("T","P",101325,"Q",0,"HEOS::"&amp;[1]!MixtureString(A16:A19,B16:B19))</f>
-        <v>78.650190680028572</v>
+        <v>78.933403642237366</v>
       </c>
       <c r="D20">
-        <v>78.650190680028572</v>
+        <v>78.933403642237366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unprotect Example wkbk and rename VBA to CoolProp
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -5273,7 +5273,7 @@
   <dimension ref="B1:J38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5478,7 +5478,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="E1:H4"/>
     <mergeCell ref="I1:J4"/>
@@ -6107,7 +6107,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="C1:F4"/>
     <mergeCell ref="C5:F5"/>
@@ -7467,7 +7466,6 @@
       <c r="I46" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="B2:H2"/>
   </mergeCells>
@@ -7743,7 +7741,7 @@
       <c r="H21" s="49"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="C4:E4"/>
   </mergeCells>
@@ -9832,7 +9830,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="4">

</xml_diff>

<commit_message>
Removed the absolute path from the Excel example file
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" updateLinks="always" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Installation" sheetId="3" r:id="rId1"/>
@@ -13,26 +13,23 @@
     <sheet name="Property Calculator" sheetId="5" r:id="rId4"/>
     <sheet name="Lists" sheetId="4" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <definedNames>
     <definedName name="FluidType">Lists!$J$6:$J$7</definedName>
     <definedName name="ParameterList">Lists!$H$6:$H$170</definedName>
     <definedName name="PredefinedMixtures">Lists!$F$6:$F$110</definedName>
     <definedName name="PureFluids">Lists!$D$6:$D$127</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Forfatter</author>
   </authors>
   <commentList>
-    <comment ref="D13" authorId="0" shapeId="0">
+    <comment ref="D13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -42,7 +39,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Forfatter:</t>
         </r>
         <r>
           <rPr>
@@ -2083,7 +2080,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -2765,7 +2762,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -2783,7 +2779,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -2801,7 +2796,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -2819,7 +2813,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -2837,9 +2830,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2871,6 +2864,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2912,121 +2906,121 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>6.1220367642211804E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.021255884870882</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83.914144952818432</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>125.73397341918556</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>167.53303558721041</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>209.34176132668063</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>251.18035191397172</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>293.06519282229556</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>335.01235325255885</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>377.0393864777609</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>419.16616289289357</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>461.41518953432495</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>503.8116924214724</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>546.38362438115018</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>589.16169048823451</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>632.17944178057041</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>675.47346558322567</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>719.08369096295519</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>763.05382639582695</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>807.43195145025004</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>852.27129446018171</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>897.63124444416758</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>943.5786700422434</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>990.18965507747316</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1037.5518165790293</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1085.7674588110542</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1134.9579569891273</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1185.2699943566115</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1236.8846659592693</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1290.0311497479684</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1345.0079264161159</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1402.2171260009679</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1462.2236463970921</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1525.8683270550669</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1594.528992236294</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1670.8899067278082</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1761.6646205355523</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1890.6872488661777</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2084.2562559079452</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3038,127 +3032,127 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0.61165475093481403</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2281989483882039</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3393181786436497</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2469708331101756</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.384938072463564</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.351945830311132</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.94643430777359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.200930028016629</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.414474031259203</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.181765816481359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.4179966597451</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.37871294870251</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198.67442047982439</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>270.27997678494478</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>361.53909939949972</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>476.16453797107482</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>618.23462142573601</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>792.18700698159432</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1002.8105360789027</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1255.2361551604806</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1554.9279004664593</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1907.6749935327782</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2319.5861702580783</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2797.0874969305182</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3346.9251442691766</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3976.1749306527868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4692.260992299477</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5502.9867830144822</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6416.5829095313811</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7441.7783444211764</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8587.9049408351511</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9865.051211181868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11284.292927464998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12858.051600204844</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14600.677372002267</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16529.415139051383</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18666.006646276372</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21043.563147465797</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22064</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-A75F-498C-BF29-0884D82DF471}"/>
             </c:ext>
@@ -3187,121 +3181,121 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>2500.9151916490414</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2519.2083189072159</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2537.433404372583</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2555.5452032947655</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2573.510322374003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2591.2888878672011</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2608.834872217727</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2626.0964008315264</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2643.0158813452144</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2659.5300141957373</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2675.5698844194585</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2691.0613426859559</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2705.925765793183</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2720.0811051450492</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2733.4429731737537</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2745.9254514300692</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2757.4413489920948</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2767.9017622614256</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2777.2149260215888</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2785.28444476203</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2792.0070226267226</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2797.2697683428009</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2800.9470527725625</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2802.8967584010443</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2802.9556046252333</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2800.9330729758299</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2796.6032203853515</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2789.6932193000116</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2779.8667305294516</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2766.6990506391339</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2749.638761400251</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2727.9458789653854</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2700.5857692409359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2666.0311405571688</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2621.8455755251834</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2563.6367109445878</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2481.4924833359378</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2334.5182916068898</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2084.2562559079452</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3313,127 +3307,127 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0.61165475093481403</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2281989483882039</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3393181786436497</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2469708331101756</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.384938072463564</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.351945830311132</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.94643430777359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.200930028016629</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.414474031259203</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.181765816481359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.4179966597451</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.37871294870251</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198.67442047982439</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>270.27997678494478</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>361.53909939949972</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>476.16453797107482</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>618.23462142573601</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>792.18700698159432</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1002.8105360789027</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1255.2361551604806</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1554.9279004664593</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1907.6749935327782</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2319.5861702580783</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2797.0874969305182</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3346.9251442691766</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3976.1749306527868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4692.260992299477</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5502.9867830144822</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6416.5829095313811</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7441.7783444211764</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8587.9049408351511</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9865.051211181868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11284.292927464998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12858.051600204844</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14600.677372002267</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16529.415139051383</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18666.006646276372</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21043.563147465797</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22064</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-A75F-498C-BF29-0884D82DF471}"/>
             </c:ext>
@@ -3447,11 +3441,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123128448"/>
-        <c:axId val="125776640"/>
+        <c:axId val="268211264"/>
+        <c:axId val="268211840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123128448"/>
+        <c:axId val="268211264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3473,18 +3467,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125776640"/>
+        <c:crossAx val="268211840"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125776640"/>
+        <c:axId val="268211840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3507,13 +3502,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123128448"/>
+        <c:crossAx val="268211264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3559,9 +3555,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3593,6 +3589,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3634,121 +3631,121 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>999.79252003841918</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>999.65462464161249</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>998.16180134316721</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>995.60617747384481</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>992.17511534129687</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>987.99621061116648</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>983.16021717833735</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>977.73365598192891</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>971.76621871051191</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>965.29532855043863</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>958.3490516048596</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>950.94800358896453</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>943.10661743025366</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>934.83398660708008</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>926.13441329112538</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>917.00773926892612</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>907.44950563407372</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>897.45096587597254</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>886.99896128082094</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>876.07565429885767</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>864.65810228712633</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>852.71763851005767</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>840.2190067501075</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>827.11916655180153</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>813.36564216909869</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>798.8942202204222</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>783.62569286973462</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>767.46116679898171</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>750.27516129988146</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>731.90519964368571</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>712.13563881961386</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>690.67154560984454</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>667.09384803259582</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>640.77321526639594</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>610.66759832540311</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>574.70651653764321</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>527.59162942229307</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>451.42564747531435</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>322.00000000000006</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3760,127 +3757,127 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0.61165475093481403</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2281989483882039</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3393181786436497</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2469708331101756</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.384938072463564</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.351945830311132</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.94643430777359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.200930028016629</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.414474031259203</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.181765816481359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.4179966597451</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.37871294870251</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198.67442047982439</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>270.27997678494478</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>361.53909939949972</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>476.16453797107482</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>618.23462142573601</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>792.18700698159432</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1002.8105360789027</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1255.2361551604806</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1554.9279004664593</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1907.6749935327782</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2319.5861702580783</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2797.0874969305182</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3346.9251442691766</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3976.1749306527868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4692.260992299477</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5502.9867830144822</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6416.5829095313811</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7441.7783444211764</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8587.9049408351511</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9865.051211181868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11284.292927464998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12858.051600204844</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14600.677372002267</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16529.415139051383</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18666.006646276372</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21043.563147465797</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22064</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-849E-4AA0-9B02-6B428CC15733}"/>
             </c:ext>
@@ -3909,121 +3906,121 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>4.8545757582904008E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.4070520080232669E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7314008205457629E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0415211808981719E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1242255801689618E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.314684280044507E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13042522259659944</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.19843073794198388</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.29367213474310461</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.42389794463211244</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.59816979192617947</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.82692959572362479</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1220671917645235</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.4969959714828946</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9667450045126416</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5480771470967372</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2596441977624346</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.1221925343385504</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.1588361289208002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.3954187812092966</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.8609945167845119</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.5884655414268227</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.61543287429496</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13.98533895750843</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>16.74901930160329</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>19.966840438464878</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>23.711700367712318</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28.073335624424267</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>33.164674054046102</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>39.131512960158567</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>46.167849523793997</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>54.541361541638288</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>64.638432419886115</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>77.050425987313361</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>92.75878250741664</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>113.60561050162258</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>143.89841140849438</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>201.83931641741896</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>322.00000000000006</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4035,127 +4032,127 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0.61165475093481403</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2281989483882039</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3393181786436497</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2469708331101756</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.384938072463564</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.351945830311132</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.94643430777359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.200930028016629</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.414474031259203</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.181765816481359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.4179966597451</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.37871294870251</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198.67442047982439</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>270.27997678494478</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>361.53909939949972</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>476.16453797107482</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>618.23462142573601</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>792.18700698159432</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1002.8105360789027</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1255.2361551604806</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1554.9279004664593</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1907.6749935327782</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2319.5861702580783</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2797.0874969305182</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3346.9251442691766</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3976.1749306527868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4692.260992299477</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5502.9867830144822</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6416.5829095313811</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7441.7783444211764</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8587.9049408351511</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9865.051211181868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11284.292927464998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12858.051600204844</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14600.677372002267</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16529.415139051383</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18666.006646276372</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21043.563147465797</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22064</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-849E-4AA0-9B02-6B428CC15733}"/>
             </c:ext>
@@ -4169,11 +4166,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123128448"/>
-        <c:axId val="125776640"/>
+        <c:axId val="268213568"/>
+        <c:axId val="276922368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123128448"/>
+        <c:axId val="268213568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4195,18 +4192,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125776640"/>
+        <c:crossAx val="276922368"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125776640"/>
+        <c:axId val="276922368"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4229,13 +4227,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123128448"/>
+        <c:crossAx val="268213568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4281,9 +4280,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4311,6 +4310,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4456,7 +4456,7 @@
                   <c:v>643.15</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="General">
-                  <c:v>647.096</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4468,127 +4468,127 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>0.61165475093481403</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2281989483882039</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3393181786436497</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2469708331101756</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.384938072463564</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.351945830311132</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.94643430777359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.200930028016629</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47.414474031259203</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.181765816481359</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.4179966597451</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.37871294870251</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198.67442047982439</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>270.27997678494478</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>361.53909939949972</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>476.16453797107482</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>618.23462142573601</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>792.18700698159432</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1002.8105360789027</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1255.2361551604806</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1554.9279004664593</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1907.6749935327782</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2319.5861702580783</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2797.0874969305182</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3346.9251442691766</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3976.1749306527868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4692.260992299477</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5502.9867830144822</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6416.5829095313811</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7441.7783444211764</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8587.9049408351511</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9865.051211181868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11284.292927464998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12858.051600204844</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14600.677372002267</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16529.415139051383</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18666.006646276372</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21043.563147465797</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22064</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-28D3-4486-9E09-DF263A54D400}"/>
             </c:ext>
@@ -4602,11 +4602,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123128448"/>
-        <c:axId val="125776640"/>
+        <c:axId val="276924096"/>
+        <c:axId val="276924672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123128448"/>
+        <c:axId val="276924096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200"/>
@@ -4629,18 +4629,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125776640"/>
+        <c:crossAx val="276924672"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125776640"/>
+        <c:axId val="276924672"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4663,13 +4664,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123128448"/>
+        <c:crossAx val="276924096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4883,31 +4885,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sample calcs"/>
-      <sheetName val="Water saturation table"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="get_global_param_string"/>
-      <definedName name="HAPropsSI"/>
-      <definedName name="MixtureString"/>
-      <definedName name="PhaseSI"/>
-      <definedName name="Props1SI"/>
-      <definedName name="PropsSI"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D5:D127" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="D5:D127"/>
@@ -4949,9 +4926,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kontortema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kontor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4989,9 +4966,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kontor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5024,26 +5001,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5076,26 +5036,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kontor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5272,14 +5215,14 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:J38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="2" max="3" width="3.625" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5494,20 +5437,20 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:H46"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
+    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.125" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.42578125" customWidth="1"/>
-    <col min="8" max="8" width="72.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.375" customWidth="1"/>
+    <col min="8" max="8" width="72.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
@@ -5570,9 +5513,9 @@
       <c r="C8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="25">
-        <f>[1]!Props1SI("R410A","Tcrit")</f>
-        <v>344.49400000000003</v>
+      <c r="D8" s="25" t="e">
+        <f ca="1">Props1SI("R410A","Tcrit")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="23">
@@ -5589,9 +5532,9 @@
       <c r="C9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="25">
-        <f>[1]!Props1SI("Propane","rhocrit")</f>
-        <v>220.47810000000004</v>
+      <c r="D9" s="25" t="e">
+        <f ca="1">Props1SI("Propane","rhocrit")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="23">
@@ -5608,9 +5551,9 @@
       <c r="C10" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="25">
-        <f>[1]!PropsSI("Dmass","T",273.15,"P",101325,"HEOS::Nitrogen")</f>
-        <v>1.2503861303389008</v>
+      <c r="D10" s="25" t="e">
+        <f ca="1">PropsSI("Dmass","T",273.15,"P",101325,"HEOS::Nitrogen")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="23">
@@ -5627,9 +5570,9 @@
       <c r="C11" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="25">
-        <f>[1]!PropsSI("Dmass","T",273.15,"P",101325,"HEOS::Air")</f>
-        <v>1.2930656163292635</v>
+      <c r="D11" s="25" t="e">
+        <f ca="1">PropsSI("Dmass","T",273.15,"P",101325,"HEOS::Air")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E11" s="28"/>
       <c r="F11" s="23">
@@ -5646,9 +5589,9 @@
       <c r="C12" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="25">
-        <f>[1]!PropsSI("T","P",101325,"Q",0,"HEOS::Water")-273.15</f>
-        <v>99.974295847684004</v>
+      <c r="D12" s="25" t="e">
+        <f ca="1">PropsSI("T","P",101325,"Q",0,"HEOS::Water")-273.15</f>
+        <v>#NAME?</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="23">
@@ -5666,8 +5609,8 @@
         <v>7</v>
       </c>
       <c r="D13" s="25" t="e">
-        <f>[1]!PropsSI("T","P",101325,"Q",0,"REFPROP::Water")-273.15</f>
-        <v>#VALUE!</v>
+        <f ca="1">PropsSI("T","P",101325,"Q",0,"REFPROP::Water")-273.15</f>
+        <v>#NAME?</v>
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="23">
@@ -5682,9 +5625,9 @@
         <v>15</v>
       </c>
       <c r="C14" s="24"/>
-      <c r="D14" s="35" t="str">
-        <f>[1]!Props1SI("A","B")</f>
-        <v>Neither input to Props1SI [A,B] is a valid fluid</v>
+      <c r="D14" s="35" t="e">
+        <f ca="1">Props1SI("A","B")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="23"/>
@@ -5697,9 +5640,9 @@
         <v>94</v>
       </c>
       <c r="C15" s="26"/>
-      <c r="D15" s="25" t="str">
-        <f>[1]!get_global_param_string("version")</f>
-        <v>6.0.0</v>
+      <c r="D15" s="25" t="e">
+        <f ca="1">get_global_param_string("version")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E15" s="28"/>
       <c r="F15" s="40" t="s">
@@ -5714,9 +5657,9 @@
         <v>95</v>
       </c>
       <c r="C16" s="26"/>
-      <c r="D16" s="27" t="str">
-        <f>[1]!get_global_param_string("gitrevision")</f>
-        <v>df13df7756aa9352c56ef6f8d631365be590533c</v>
+      <c r="D16" s="27" t="e">
+        <f ca="1">get_global_param_string("gitrevision")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="23"/>
@@ -5738,9 +5681,9 @@
         <v>78</v>
       </c>
       <c r="C19" s="24"/>
-      <c r="D19" s="25" t="str">
-        <f>[1]!PhaseSI("T",293.15,"P",101325,"Water")</f>
-        <v>liquid</v>
+      <c r="D19" s="25" t="e">
+        <f ca="1">PhaseSI("T",293.15,"P",101325,"Water")</f>
+        <v>#NAME?</v>
       </c>
       <c r="F19" s="40" t="s">
         <v>79</v>
@@ -5754,9 +5697,9 @@
         <v>81</v>
       </c>
       <c r="C20" s="24"/>
-      <c r="D20" s="25" t="str">
-        <f>[1]!PhaseSI("T",400,"P",101325,"Water")</f>
-        <v>gas</v>
+      <c r="D20" s="25" t="e">
+        <f ca="1">PhaseSI("T",400,"P",101325,"Water")</f>
+        <v>#NAME?</v>
       </c>
       <c r="F20" s="40" t="s">
         <v>82</v>
@@ -5770,9 +5713,9 @@
         <v>87</v>
       </c>
       <c r="C21" s="24"/>
-      <c r="D21" s="25" t="str">
-        <f>[1]!PhaseSI("T",400,"P",30000000,"Water")</f>
-        <v>supercritical_liquid</v>
+      <c r="D21" s="25" t="e">
+        <f ca="1">PhaseSI("T",400,"P",30000000,"Water")</f>
+        <v>#NAME?</v>
       </c>
       <c r="F21" s="40" t="s">
         <v>85</v>
@@ -5786,9 +5729,9 @@
         <v>88</v>
       </c>
       <c r="C22" s="24"/>
-      <c r="D22" s="25" t="str">
-        <f>[1]!PhaseSI("T",1030,"P",10000000,"Water")</f>
-        <v>supercritical_gas</v>
+      <c r="D22" s="25" t="e">
+        <f ca="1">PhaseSI("T",1030,"P",10000000,"Water")</f>
+        <v>#NAME?</v>
       </c>
       <c r="F22" s="40" t="s">
         <v>86</v>
@@ -5802,9 +5745,9 @@
         <v>89</v>
       </c>
       <c r="C23" s="24"/>
-      <c r="D23" s="25" t="str">
-        <f>[1]!PhaseSI("T",1030,"P",30000000,"Water")</f>
-        <v>supercritical</v>
+      <c r="D23" s="25" t="e">
+        <f ca="1">PhaseSI("T",1030,"P",30000000,"Water")</f>
+        <v>#NAME?</v>
       </c>
       <c r="F23" s="40" t="s">
         <v>90</v>
@@ -5868,9 +5811,9 @@
       <c r="C31" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="25">
-        <f>[1]!PropsSI("T","P",101325,"Q",0,"HEOS::"&amp;[1]!MixtureString(B27:B30,C27:C30))</f>
-        <v>78.933406066580631</v>
+      <c r="D31" s="25" t="e">
+        <f ca="1">PropsSI("T","P",101325,"Q",0,"HEOS::"&amp;MixtureString(B27:B30,C27:C30))</f>
+        <v>#NAME?</v>
       </c>
       <c r="F31" s="25">
         <v>78.933403642237366</v>
@@ -5886,9 +5829,9 @@
       <c r="C32" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="23">
-        <f>[1]!PropsSI("D","T",273.15,"P",101325,"HEOS::"&amp;[1]!MixtureString(B27:B30,C27:C30))</f>
-        <v>1.2931619537014851</v>
+      <c r="D32" s="23" t="e">
+        <f ca="1">PropsSI("D","T",273.15,"P",101325,"HEOS::"&amp;MixtureString(B27:B30,C27:C30))</f>
+        <v>#NAME?</v>
       </c>
       <c r="F32" s="23">
         <v>1.2931619537014851</v>
@@ -5923,9 +5866,9 @@
       <c r="C35" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="25">
-        <f>[1]!HAPropsSI("D","T",293.15,"P",101325,"R",0)</f>
-        <v>149.39544393636223</v>
+      <c r="D35" s="25" t="e">
+        <f ca="1">HAPropsSI("D","T",293.15,"P",101325,"R",0)</f>
+        <v>#NAME?</v>
       </c>
       <c r="F35" s="25">
         <v>149.39544393636223</v>
@@ -5941,9 +5884,9 @@
       <c r="C36" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="25">
-        <f>[1]!HAPropsSI("D","T",293.15,"P",101325,"R",0.5)</f>
-        <v>282.42442581501291</v>
+      <c r="D36" s="25" t="e">
+        <f ca="1">HAPropsSI("D","T",293.15,"P",101325,"R",0.5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="F36" s="25">
         <v>282.42442581501291</v>
@@ -5959,9 +5902,9 @@
       <c r="C37" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="25">
-        <f>1/[1]!HAPropsSI("Vda","T",273.15,"P",101325,"R",0)</f>
-        <v>1.2930956154536004</v>
+      <c r="D37" s="25" t="e">
+        <f ca="1">1/HAPropsSI("Vda","T",273.15,"P",101325,"R",0)</f>
+        <v>#NAME?</v>
       </c>
       <c r="F37" s="25">
         <v>1.2930956154536004</v>
@@ -5977,9 +5920,9 @@
       <c r="C38" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="25">
-        <f>1/[1]!HAPropsSI("Vha","T",273.15,"P",101325,"R",0.5)</f>
-        <v>1.2916247681318624</v>
+      <c r="D38" s="25" t="e">
+        <f ca="1">1/HAPropsSI("Vha","T",273.15,"P",101325,"R",0.5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="F38" s="25">
         <v>1.2916247681318624</v>
@@ -5995,9 +5938,9 @@
       <c r="C39" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="25">
-        <f>[1]!HAPropsSI("H","T",273.15,"P",101325,"R",0.5)</f>
-        <v>4723.4366339628559</v>
+      <c r="D39" s="25" t="e">
+        <f ca="1">HAPropsSI("H","T",273.15,"P",101325,"R",0.5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="F39" s="25">
         <v>4723.4366339628559</v>
@@ -6007,16 +5950,16 @@
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="str">
-        <f>"Temperature of Sat. Air at H="&amp;TEXT(D39,"0.00")&amp;" J/kg:"</f>
-        <v>Temperature of Sat. Air at H=4723.44 J/kg:</v>
+      <c r="B40" s="23" t="e">
+        <f ca="1">"Temperature of Sat. Air at H="&amp;TEXT(D39,"0.00")&amp;" J/kg:"</f>
+        <v>#NAME?</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="25">
-        <f>[1]!HAPropsSI("T","H",D39,"P",101325,"R",1)</f>
-        <v>270.38566397315532</v>
+      <c r="D40" s="25" t="e">
+        <f ca="1">HAPropsSI("T","H",D39,"P",101325,"R",1)</f>
+        <v>#NAME?</v>
       </c>
       <c r="F40" s="25">
         <v>270.38566397315532</v>
@@ -6056,9 +5999,9 @@
       <c r="C44" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="25">
-        <f>[1]!PropsSI("V","T",300,"P",101325,"INCOMP::MEG[0.2]")</f>
-        <v>1.3814221664421487E-3</v>
+      <c r="D44" s="25" t="e">
+        <f ca="1">PropsSI("V","T",300,"P",101325,"INCOMP::MEG[0.2]")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E44" s="28"/>
       <c r="F44" s="23">
@@ -6075,9 +6018,9 @@
       <c r="C45" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="25">
-        <f>[1]!PropsSI("C","T",500,"P",101325,"INCOMP::DowQ")</f>
-        <v>2288.1643758645673</v>
+      <c r="D45" s="25" t="e">
+        <f ca="1">PropsSI("C","T",500,"P",101325,"INCOMP::DowQ")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E45" s="28"/>
       <c r="F45" s="23">
@@ -6094,9 +6037,9 @@
       <c r="C46" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="25">
-        <f>[1]!PropsSI("D","T",293.15,"P",101325,"INCOMP::MITSW[0.035]")</f>
-        <v>1024.8598443641281</v>
+      <c r="D46" s="25" t="e">
+        <f ca="1">PropsSI("D","T",293.15,"P",101325,"INCOMP::MITSW[0.035]")</f>
+        <v>#NAME?</v>
       </c>
       <c r="E46" s="28"/>
       <c r="F46" s="23">
@@ -6130,14 +6073,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" customWidth="1"/>
+    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.25" customWidth="1"/>
+    <col min="6" max="6" width="11.375" customWidth="1"/>
+    <col min="7" max="7" width="12.75" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" customWidth="1"/>
+    <col min="9" max="9" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6253,25 +6196,25 @@
         <f>B7+273.15</f>
         <v>273.16000009999999</v>
       </c>
-      <c r="D7" s="6">
-        <f>[1]!PropsSI("P","T",C7,"Q",1,"Water")/1000</f>
-        <v>0.61165475093481403</v>
-      </c>
-      <c r="E7" s="7">
-        <f>[1]!PropsSI("D","T",$C7,"Q",0,"Water")</f>
-        <v>999.79252003841918</v>
-      </c>
-      <c r="F7" s="7">
-        <f>[1]!PropsSI("D","T",$C7,"Q",1,"Water")</f>
-        <v>4.8545757582904008E-3</v>
-      </c>
-      <c r="G7" s="5">
-        <f>[1]!PropsSI("H","T",$C7,"Q",0,"Water")/1000</f>
-        <v>6.1220367642211804E-4</v>
-      </c>
-      <c r="H7" s="15">
-        <f>[1]!PropsSI("H","T",$C7,"Q",1,"Water")/1000</f>
-        <v>2500.9151916490414</v>
+      <c r="D7" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C7,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E7" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C7,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F7" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C7,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G7" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C7,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H7" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C7,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -6284,25 +6227,25 @@
         <f t="shared" ref="C8:C44" si="0">B8+273.15</f>
         <v>283.14999999999998</v>
       </c>
-      <c r="D8" s="6">
-        <f>[1]!PropsSI("P","T",C8,"Q",1,"Water")/1000</f>
-        <v>1.2281989483882039</v>
-      </c>
-      <c r="E8" s="7">
-        <f>[1]!PropsSI("D","T",$C8,"Q",0,"Water")</f>
-        <v>999.65462464161249</v>
-      </c>
-      <c r="F8" s="7">
-        <f>[1]!PropsSI("D","T",$C8,"Q",1,"Water")</f>
-        <v>9.4070520080232669E-3</v>
-      </c>
-      <c r="G8" s="5">
-        <f>[1]!PropsSI("H","T",$C8,"Q",0,"Water")/1000</f>
-        <v>42.021255884870882</v>
-      </c>
-      <c r="H8" s="15">
-        <f>[1]!PropsSI("H","T",$C8,"Q",1,"Water")/1000</f>
-        <v>2519.2083189072159</v>
+      <c r="D8" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C8,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E8" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C8,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F8" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C8,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G8" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C8,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H8" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C8,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -6315,25 +6258,25 @@
         <f t="shared" si="0"/>
         <v>293.14999999999998</v>
       </c>
-      <c r="D9" s="6">
-        <f>[1]!PropsSI("P","T",C9,"Q",1,"Water")/1000</f>
-        <v>2.3393181786436497</v>
-      </c>
-      <c r="E9" s="7">
-        <f>[1]!PropsSI("D","T",$C9,"Q",0,"Water")</f>
-        <v>998.16180134316721</v>
-      </c>
-      <c r="F9" s="7">
-        <f>[1]!PropsSI("D","T",$C9,"Q",1,"Water")</f>
-        <v>1.7314008205457629E-2</v>
-      </c>
-      <c r="G9" s="5">
-        <f>[1]!PropsSI("H","T",$C9,"Q",0,"Water")/1000</f>
-        <v>83.914144952818432</v>
-      </c>
-      <c r="H9" s="15">
-        <f>[1]!PropsSI("H","T",$C9,"Q",1,"Water")/1000</f>
-        <v>2537.433404372583</v>
+      <c r="D9" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C9,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E9" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C9,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F9" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C9,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G9" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C9,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H9" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C9,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -6346,25 +6289,25 @@
         <f t="shared" si="0"/>
         <v>303.14999999999998</v>
       </c>
-      <c r="D10" s="6">
-        <f>[1]!PropsSI("P","T",C10,"Q",1,"Water")/1000</f>
-        <v>4.2469708331101756</v>
-      </c>
-      <c r="E10" s="7">
-        <f>[1]!PropsSI("D","T",$C10,"Q",0,"Water")</f>
-        <v>995.60617747384481</v>
-      </c>
-      <c r="F10" s="7">
-        <f>[1]!PropsSI("D","T",$C10,"Q",1,"Water")</f>
-        <v>3.0415211808981719E-2</v>
-      </c>
-      <c r="G10" s="5">
-        <f>[1]!PropsSI("H","T",$C10,"Q",0,"Water")/1000</f>
-        <v>125.73397341918556</v>
-      </c>
-      <c r="H10" s="15">
-        <f>[1]!PropsSI("H","T",$C10,"Q",1,"Water")/1000</f>
-        <v>2555.5452032947655</v>
+      <c r="D10" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C10,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E10" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C10,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F10" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C10,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G10" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C10,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H10" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C10,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I10" s="1"/>
     </row>
@@ -6377,25 +6320,25 @@
         <f t="shared" si="0"/>
         <v>313.14999999999998</v>
       </c>
-      <c r="D11" s="6">
-        <f>[1]!PropsSI("P","T",C11,"Q",1,"Water")/1000</f>
-        <v>7.384938072463564</v>
-      </c>
-      <c r="E11" s="7">
-        <f>[1]!PropsSI("D","T",$C11,"Q",0,"Water")</f>
-        <v>992.17511534129687</v>
-      </c>
-      <c r="F11" s="7">
-        <f>[1]!PropsSI("D","T",$C11,"Q",1,"Water")</f>
-        <v>5.1242255801689618E-2</v>
-      </c>
-      <c r="G11" s="5">
-        <f>[1]!PropsSI("H","T",$C11,"Q",0,"Water")/1000</f>
-        <v>167.53303558721041</v>
-      </c>
-      <c r="H11" s="15">
-        <f>[1]!PropsSI("H","T",$C11,"Q",1,"Water")/1000</f>
-        <v>2573.510322374003</v>
+      <c r="D11" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C11,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E11" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C11,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F11" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C11,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G11" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C11,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H11" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C11,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -6408,25 +6351,25 @@
         <f t="shared" si="0"/>
         <v>323.14999999999998</v>
       </c>
-      <c r="D12" s="6">
-        <f>[1]!PropsSI("P","T",C12,"Q",1,"Water")/1000</f>
-        <v>12.351945830311132</v>
-      </c>
-      <c r="E12" s="7">
-        <f>[1]!PropsSI("D","T",$C12,"Q",0,"Water")</f>
-        <v>987.99621061116648</v>
-      </c>
-      <c r="F12" s="7">
-        <f>[1]!PropsSI("D","T",$C12,"Q",1,"Water")</f>
-        <v>8.314684280044507E-2</v>
-      </c>
-      <c r="G12" s="5">
-        <f>[1]!PropsSI("H","T",$C12,"Q",0,"Water")/1000</f>
-        <v>209.34176132668063</v>
-      </c>
-      <c r="H12" s="15">
-        <f>[1]!PropsSI("H","T",$C12,"Q",1,"Water")/1000</f>
-        <v>2591.2888878672011</v>
+      <c r="D12" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C12,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E12" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C12,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F12" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C12,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G12" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C12,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H12" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C12,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -6439,25 +6382,25 @@
         <f t="shared" si="0"/>
         <v>333.15</v>
       </c>
-      <c r="D13" s="6">
-        <f>[1]!PropsSI("P","T",C13,"Q",1,"Water")/1000</f>
-        <v>19.94643430777359</v>
-      </c>
-      <c r="E13" s="7">
-        <f>[1]!PropsSI("D","T",$C13,"Q",0,"Water")</f>
-        <v>983.16021717833735</v>
-      </c>
-      <c r="F13" s="7">
-        <f>[1]!PropsSI("D","T",$C13,"Q",1,"Water")</f>
-        <v>0.13042522259659944</v>
-      </c>
-      <c r="G13" s="5">
-        <f>[1]!PropsSI("H","T",$C13,"Q",0,"Water")/1000</f>
-        <v>251.18035191397172</v>
-      </c>
-      <c r="H13" s="15">
-        <f>[1]!PropsSI("H","T",$C13,"Q",1,"Water")/1000</f>
-        <v>2608.834872217727</v>
+      <c r="D13" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C13,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E13" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C13,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F13" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C13,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G13" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C13,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H13" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C13,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -6470,25 +6413,25 @@
         <f t="shared" si="0"/>
         <v>343.15</v>
       </c>
-      <c r="D14" s="6">
-        <f>[1]!PropsSI("P","T",C14,"Q",1,"Water")/1000</f>
-        <v>31.200930028016629</v>
-      </c>
-      <c r="E14" s="7">
-        <f>[1]!PropsSI("D","T",$C14,"Q",0,"Water")</f>
-        <v>977.73365598192891</v>
-      </c>
-      <c r="F14" s="7">
-        <f>[1]!PropsSI("D","T",$C14,"Q",1,"Water")</f>
-        <v>0.19843073794198388</v>
-      </c>
-      <c r="G14" s="5">
-        <f>[1]!PropsSI("H","T",$C14,"Q",0,"Water")/1000</f>
-        <v>293.06519282229556</v>
-      </c>
-      <c r="H14" s="15">
-        <f>[1]!PropsSI("H","T",$C14,"Q",1,"Water")/1000</f>
-        <v>2626.0964008315264</v>
+      <c r="D14" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C14,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E14" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C14,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F14" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C14,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G14" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C14,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H14" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C14,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -6501,25 +6444,25 @@
         <f t="shared" si="0"/>
         <v>353.15</v>
       </c>
-      <c r="D15" s="6">
-        <f>[1]!PropsSI("P","T",C15,"Q",1,"Water")/1000</f>
-        <v>47.414474031259203</v>
-      </c>
-      <c r="E15" s="7">
-        <f>[1]!PropsSI("D","T",$C15,"Q",0,"Water")</f>
-        <v>971.76621871051191</v>
-      </c>
-      <c r="F15" s="7">
-        <f>[1]!PropsSI("D","T",$C15,"Q",1,"Water")</f>
-        <v>0.29367213474310461</v>
-      </c>
-      <c r="G15" s="5">
-        <f>[1]!PropsSI("H","T",$C15,"Q",0,"Water")/1000</f>
-        <v>335.01235325255885</v>
-      </c>
-      <c r="H15" s="15">
-        <f>[1]!PropsSI("H","T",$C15,"Q",1,"Water")/1000</f>
-        <v>2643.0158813452144</v>
+      <c r="D15" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C15,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E15" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C15,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F15" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C15,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G15" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C15,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H15" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C15,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -6532,25 +6475,25 @@
         <f t="shared" si="0"/>
         <v>363.15</v>
       </c>
-      <c r="D16" s="6">
-        <f>[1]!PropsSI("P","T",C16,"Q",1,"Water")/1000</f>
-        <v>70.181765816481359</v>
-      </c>
-      <c r="E16" s="7">
-        <f>[1]!PropsSI("D","T",$C16,"Q",0,"Water")</f>
-        <v>965.29532855043863</v>
-      </c>
-      <c r="F16" s="7">
-        <f>[1]!PropsSI("D","T",$C16,"Q",1,"Water")</f>
-        <v>0.42389794463211244</v>
-      </c>
-      <c r="G16" s="5">
-        <f>[1]!PropsSI("H","T",$C16,"Q",0,"Water")/1000</f>
-        <v>377.0393864777609</v>
-      </c>
-      <c r="H16" s="15">
-        <f>[1]!PropsSI("H","T",$C16,"Q",1,"Water")/1000</f>
-        <v>2659.5300141957373</v>
+      <c r="D16" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C16,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E16" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C16,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F16" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C16,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G16" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C16,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H16" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C16,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -6563,25 +6506,25 @@
         <f t="shared" si="0"/>
         <v>373.15</v>
       </c>
-      <c r="D17" s="6">
-        <f>[1]!PropsSI("P","T",C17,"Q",1,"Water")/1000</f>
-        <v>101.4179966597451</v>
-      </c>
-      <c r="E17" s="7">
-        <f>[1]!PropsSI("D","T",$C17,"Q",0,"Water")</f>
-        <v>958.3490516048596</v>
-      </c>
-      <c r="F17" s="7">
-        <f>[1]!PropsSI("D","T",$C17,"Q",1,"Water")</f>
-        <v>0.59816979192617947</v>
-      </c>
-      <c r="G17" s="5">
-        <f>[1]!PropsSI("H","T",$C17,"Q",0,"Water")/1000</f>
-        <v>419.16616289289357</v>
-      </c>
-      <c r="H17" s="15">
-        <f>[1]!PropsSI("H","T",$C17,"Q",1,"Water")/1000</f>
-        <v>2675.5698844194585</v>
+      <c r="D17" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C17,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E17" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C17,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F17" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C17,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G17" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C17,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H17" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C17,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -6594,25 +6537,25 @@
         <f t="shared" si="0"/>
         <v>383.15</v>
       </c>
-      <c r="D18" s="6">
-        <f>[1]!PropsSI("P","T",C18,"Q",1,"Water")/1000</f>
-        <v>143.37871294870251</v>
-      </c>
-      <c r="E18" s="7">
-        <f>[1]!PropsSI("D","T",$C18,"Q",0,"Water")</f>
-        <v>950.94800358896453</v>
-      </c>
-      <c r="F18" s="7">
-        <f>[1]!PropsSI("D","T",$C18,"Q",1,"Water")</f>
-        <v>0.82692959572362479</v>
-      </c>
-      <c r="G18" s="5">
-        <f>[1]!PropsSI("H","T",$C18,"Q",0,"Water")/1000</f>
-        <v>461.41518953432495</v>
-      </c>
-      <c r="H18" s="15">
-        <f>[1]!PropsSI("H","T",$C18,"Q",1,"Water")/1000</f>
-        <v>2691.0613426859559</v>
+      <c r="D18" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C18,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E18" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C18,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F18" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C18,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G18" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C18,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H18" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C18,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -6625,25 +6568,25 @@
         <f t="shared" si="0"/>
         <v>393.15</v>
       </c>
-      <c r="D19" s="6">
-        <f>[1]!PropsSI("P","T",C19,"Q",1,"Water")/1000</f>
-        <v>198.67442047982439</v>
-      </c>
-      <c r="E19" s="7">
-        <f>[1]!PropsSI("D","T",$C19,"Q",0,"Water")</f>
-        <v>943.10661743025366</v>
-      </c>
-      <c r="F19" s="7">
-        <f>[1]!PropsSI("D","T",$C19,"Q",1,"Water")</f>
-        <v>1.1220671917645235</v>
-      </c>
-      <c r="G19" s="5">
-        <f>[1]!PropsSI("H","T",$C19,"Q",0,"Water")/1000</f>
-        <v>503.8116924214724</v>
-      </c>
-      <c r="H19" s="15">
-        <f>[1]!PropsSI("H","T",$C19,"Q",1,"Water")/1000</f>
-        <v>2705.925765793183</v>
+      <c r="D19" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C19,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E19" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C19,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F19" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C19,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G19" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C19,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H19" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C19,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I19" s="1"/>
     </row>
@@ -6656,25 +6599,25 @@
         <f t="shared" si="0"/>
         <v>403.15</v>
       </c>
-      <c r="D20" s="6">
-        <f>[1]!PropsSI("P","T",C20,"Q",1,"Water")/1000</f>
-        <v>270.27997678494478</v>
-      </c>
-      <c r="E20" s="7">
-        <f>[1]!PropsSI("D","T",$C20,"Q",0,"Water")</f>
-        <v>934.83398660708008</v>
-      </c>
-      <c r="F20" s="7">
-        <f>[1]!PropsSI("D","T",$C20,"Q",1,"Water")</f>
-        <v>1.4969959714828946</v>
-      </c>
-      <c r="G20" s="5">
-        <f>[1]!PropsSI("H","T",$C20,"Q",0,"Water")/1000</f>
-        <v>546.38362438115018</v>
-      </c>
-      <c r="H20" s="15">
-        <f>[1]!PropsSI("H","T",$C20,"Q",1,"Water")/1000</f>
-        <v>2720.0811051450492</v>
+      <c r="D20" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C20,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E20" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C20,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F20" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C20,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G20" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C20,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H20" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C20,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -6687,25 +6630,25 @@
         <f t="shared" si="0"/>
         <v>413.15</v>
       </c>
-      <c r="D21" s="6">
-        <f>[1]!PropsSI("P","T",C21,"Q",1,"Water")/1000</f>
-        <v>361.53909939949972</v>
-      </c>
-      <c r="E21" s="7">
-        <f>[1]!PropsSI("D","T",$C21,"Q",0,"Water")</f>
-        <v>926.13441329112538</v>
-      </c>
-      <c r="F21" s="7">
-        <f>[1]!PropsSI("D","T",$C21,"Q",1,"Water")</f>
-        <v>1.9667450045126416</v>
-      </c>
-      <c r="G21" s="5">
-        <f>[1]!PropsSI("H","T",$C21,"Q",0,"Water")/1000</f>
-        <v>589.16169048823451</v>
-      </c>
-      <c r="H21" s="15">
-        <f>[1]!PropsSI("H","T",$C21,"Q",1,"Water")/1000</f>
-        <v>2733.4429731737537</v>
+      <c r="D21" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C21,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E21" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C21,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F21" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C21,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G21" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C21,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H21" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C21,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -6718,25 +6661,25 @@
         <f t="shared" si="0"/>
         <v>423.15</v>
       </c>
-      <c r="D22" s="6">
-        <f>[1]!PropsSI("P","T",C22,"Q",1,"Water")/1000</f>
-        <v>476.16453797107482</v>
-      </c>
-      <c r="E22" s="7">
-        <f>[1]!PropsSI("D","T",$C22,"Q",0,"Water")</f>
-        <v>917.00773926892612</v>
-      </c>
-      <c r="F22" s="7">
-        <f>[1]!PropsSI("D","T",$C22,"Q",1,"Water")</f>
-        <v>2.5480771470967372</v>
-      </c>
-      <c r="G22" s="5">
-        <f>[1]!PropsSI("H","T",$C22,"Q",0,"Water")/1000</f>
-        <v>632.17944178057041</v>
-      </c>
-      <c r="H22" s="15">
-        <f>[1]!PropsSI("H","T",$C22,"Q",1,"Water")/1000</f>
-        <v>2745.9254514300692</v>
+      <c r="D22" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C22,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E22" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C22,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F22" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C22,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G22" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C22,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H22" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C22,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I22" s="1"/>
     </row>
@@ -6749,25 +6692,25 @@
         <f t="shared" si="0"/>
         <v>433.15</v>
       </c>
-      <c r="D23" s="6">
-        <f>[1]!PropsSI("P","T",C23,"Q",1,"Water")/1000</f>
-        <v>618.23462142573601</v>
-      </c>
-      <c r="E23" s="7">
-        <f>[1]!PropsSI("D","T",$C23,"Q",0,"Water")</f>
-        <v>907.44950563407372</v>
-      </c>
-      <c r="F23" s="7">
-        <f>[1]!PropsSI("D","T",$C23,"Q",1,"Water")</f>
-        <v>3.2596441977624346</v>
-      </c>
-      <c r="G23" s="5">
-        <f>[1]!PropsSI("H","T",$C23,"Q",0,"Water")/1000</f>
-        <v>675.47346558322567</v>
-      </c>
-      <c r="H23" s="15">
-        <f>[1]!PropsSI("H","T",$C23,"Q",1,"Water")/1000</f>
-        <v>2757.4413489920948</v>
+      <c r="D23" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C23,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E23" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C23,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F23" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C23,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G23" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C23,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H23" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C23,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I23" s="1"/>
     </row>
@@ -6780,25 +6723,25 @@
         <f t="shared" si="0"/>
         <v>443.15</v>
       </c>
-      <c r="D24" s="6">
-        <f>[1]!PropsSI("P","T",C24,"Q",1,"Water")/1000</f>
-        <v>792.18700698159432</v>
-      </c>
-      <c r="E24" s="7">
-        <f>[1]!PropsSI("D","T",$C24,"Q",0,"Water")</f>
-        <v>897.45096587597254</v>
-      </c>
-      <c r="F24" s="7">
-        <f>[1]!PropsSI("D","T",$C24,"Q",1,"Water")</f>
-        <v>4.1221925343385504</v>
-      </c>
-      <c r="G24" s="5">
-        <f>[1]!PropsSI("H","T",$C24,"Q",0,"Water")/1000</f>
-        <v>719.08369096295519</v>
-      </c>
-      <c r="H24" s="15">
-        <f>[1]!PropsSI("H","T",$C24,"Q",1,"Water")/1000</f>
-        <v>2767.9017622614256</v>
+      <c r="D24" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C24,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E24" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C24,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F24" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C24,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G24" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C24,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H24" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C24,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -6811,25 +6754,25 @@
         <f t="shared" si="0"/>
         <v>453.15</v>
       </c>
-      <c r="D25" s="6">
-        <f>[1]!PropsSI("P","T",C25,"Q",1,"Water")/1000</f>
-        <v>1002.8105360789027</v>
-      </c>
-      <c r="E25" s="7">
-        <f>[1]!PropsSI("D","T",$C25,"Q",0,"Water")</f>
-        <v>886.99896128082094</v>
-      </c>
-      <c r="F25" s="7">
-        <f>[1]!PropsSI("D","T",$C25,"Q",1,"Water")</f>
-        <v>5.1588361289208002</v>
-      </c>
-      <c r="G25" s="5">
-        <f>[1]!PropsSI("H","T",$C25,"Q",0,"Water")/1000</f>
-        <v>763.05382639582695</v>
-      </c>
-      <c r="H25" s="15">
-        <f>[1]!PropsSI("H","T",$C25,"Q",1,"Water")/1000</f>
-        <v>2777.2149260215888</v>
+      <c r="D25" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C25,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E25" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C25,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F25" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C25,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G25" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C25,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H25" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C25,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I25" s="1"/>
     </row>
@@ -6842,25 +6785,25 @@
         <f t="shared" si="0"/>
         <v>463.15</v>
       </c>
-      <c r="D26" s="6">
-        <f>[1]!PropsSI("P","T",C26,"Q",1,"Water")/1000</f>
-        <v>1255.2361551604806</v>
-      </c>
-      <c r="E26" s="7">
-        <f>[1]!PropsSI("D","T",$C26,"Q",0,"Water")</f>
-        <v>876.07565429885767</v>
-      </c>
-      <c r="F26" s="7">
-        <f>[1]!PropsSI("D","T",$C26,"Q",1,"Water")</f>
-        <v>6.3954187812092966</v>
-      </c>
-      <c r="G26" s="5">
-        <f>[1]!PropsSI("H","T",$C26,"Q",0,"Water")/1000</f>
-        <v>807.43195145025004</v>
-      </c>
-      <c r="H26" s="15">
-        <f>[1]!PropsSI("H","T",$C26,"Q",1,"Water")/1000</f>
-        <v>2785.28444476203</v>
+      <c r="D26" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C26,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E26" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C26,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F26" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C26,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G26" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C26,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H26" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C26,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I26" s="1"/>
     </row>
@@ -6873,25 +6816,25 @@
         <f t="shared" si="0"/>
         <v>473.15</v>
       </c>
-      <c r="D27" s="6">
-        <f>[1]!PropsSI("P","T",C27,"Q",1,"Water")/1000</f>
-        <v>1554.9279004664593</v>
-      </c>
-      <c r="E27" s="7">
-        <f>[1]!PropsSI("D","T",$C27,"Q",0,"Water")</f>
-        <v>864.65810228712633</v>
-      </c>
-      <c r="F27" s="7">
-        <f>[1]!PropsSI("D","T",$C27,"Q",1,"Water")</f>
-        <v>7.8609945167845119</v>
-      </c>
-      <c r="G27" s="5">
-        <f>[1]!PropsSI("H","T",$C27,"Q",0,"Water")/1000</f>
-        <v>852.27129446018171</v>
-      </c>
-      <c r="H27" s="15">
-        <f>[1]!PropsSI("H","T",$C27,"Q",1,"Water")/1000</f>
-        <v>2792.0070226267226</v>
+      <c r="D27" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C27,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E27" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C27,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F27" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C27,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G27" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C27,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H27" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C27,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I27" s="1"/>
     </row>
@@ -6904,25 +6847,25 @@
         <f t="shared" si="0"/>
         <v>483.15</v>
       </c>
-      <c r="D28" s="6">
-        <f>[1]!PropsSI("P","T",C28,"Q",1,"Water")/1000</f>
-        <v>1907.6749935327782</v>
-      </c>
-      <c r="E28" s="7">
-        <f>[1]!PropsSI("D","T",$C28,"Q",0,"Water")</f>
-        <v>852.71763851005767</v>
-      </c>
-      <c r="F28" s="7">
-        <f>[1]!PropsSI("D","T",$C28,"Q",1,"Water")</f>
-        <v>9.5884655414268227</v>
-      </c>
-      <c r="G28" s="5">
-        <f>[1]!PropsSI("H","T",$C28,"Q",0,"Water")/1000</f>
-        <v>897.63124444416758</v>
-      </c>
-      <c r="H28" s="15">
-        <f>[1]!PropsSI("H","T",$C28,"Q",1,"Water")/1000</f>
-        <v>2797.2697683428009</v>
+      <c r="D28" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C28,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E28" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C28,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F28" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C28,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G28" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C28,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H28" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C28,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I28" s="1"/>
     </row>
@@ -6935,25 +6878,25 @@
         <f t="shared" si="0"/>
         <v>493.15</v>
       </c>
-      <c r="D29" s="6">
-        <f>[1]!PropsSI("P","T",C29,"Q",1,"Water")/1000</f>
-        <v>2319.5861702580783</v>
-      </c>
-      <c r="E29" s="7">
-        <f>[1]!PropsSI("D","T",$C29,"Q",0,"Water")</f>
-        <v>840.2190067501075</v>
-      </c>
-      <c r="F29" s="7">
-        <f>[1]!PropsSI("D","T",$C29,"Q",1,"Water")</f>
-        <v>11.61543287429496</v>
-      </c>
-      <c r="G29" s="5">
-        <f>[1]!PropsSI("H","T",$C29,"Q",0,"Water")/1000</f>
-        <v>943.5786700422434</v>
-      </c>
-      <c r="H29" s="15">
-        <f>[1]!PropsSI("H","T",$C29,"Q",1,"Water")/1000</f>
-        <v>2800.9470527725625</v>
+      <c r="D29" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C29,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E29" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C29,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F29" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C29,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G29" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C29,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H29" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C29,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -6966,25 +6909,25 @@
         <f t="shared" si="0"/>
         <v>503.15</v>
       </c>
-      <c r="D30" s="6">
-        <f>[1]!PropsSI("P","T",C30,"Q",1,"Water")/1000</f>
-        <v>2797.0874969305182</v>
-      </c>
-      <c r="E30" s="7">
-        <f>[1]!PropsSI("D","T",$C30,"Q",0,"Water")</f>
-        <v>827.11916655180153</v>
-      </c>
-      <c r="F30" s="7">
-        <f>[1]!PropsSI("D","T",$C30,"Q",1,"Water")</f>
-        <v>13.98533895750843</v>
-      </c>
-      <c r="G30" s="5">
-        <f>[1]!PropsSI("H","T",$C30,"Q",0,"Water")/1000</f>
-        <v>990.18965507747316</v>
-      </c>
-      <c r="H30" s="15">
-        <f>[1]!PropsSI("H","T",$C30,"Q",1,"Water")/1000</f>
-        <v>2802.8967584010443</v>
+      <c r="D30" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C30,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E30" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C30,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F30" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C30,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G30" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C30,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H30" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C30,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I30" s="1"/>
     </row>
@@ -6997,25 +6940,25 @@
         <f t="shared" si="0"/>
         <v>513.15</v>
       </c>
-      <c r="D31" s="6">
-        <f>[1]!PropsSI("P","T",C31,"Q",1,"Water")/1000</f>
-        <v>3346.9251442691766</v>
-      </c>
-      <c r="E31" s="7">
-        <f>[1]!PropsSI("D","T",$C31,"Q",0,"Water")</f>
-        <v>813.36564216909869</v>
-      </c>
-      <c r="F31" s="7">
-        <f>[1]!PropsSI("D","T",$C31,"Q",1,"Water")</f>
-        <v>16.74901930160329</v>
-      </c>
-      <c r="G31" s="5">
-        <f>[1]!PropsSI("H","T",$C31,"Q",0,"Water")/1000</f>
-        <v>1037.5518165790293</v>
-      </c>
-      <c r="H31" s="15">
-        <f>[1]!PropsSI("H","T",$C31,"Q",1,"Water")/1000</f>
-        <v>2802.9556046252333</v>
+      <c r="D31" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C31,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E31" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C31,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F31" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C31,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G31" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C31,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H31" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C31,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I31" s="1"/>
     </row>
@@ -7028,25 +6971,25 @@
         <f t="shared" si="0"/>
         <v>523.15</v>
       </c>
-      <c r="D32" s="6">
-        <f>[1]!PropsSI("P","T",C32,"Q",1,"Water")/1000</f>
-        <v>3976.1749306527868</v>
-      </c>
-      <c r="E32" s="7">
-        <f>[1]!PropsSI("D","T",$C32,"Q",0,"Water")</f>
-        <v>798.8942202204222</v>
-      </c>
-      <c r="F32" s="7">
-        <f>[1]!PropsSI("D","T",$C32,"Q",1,"Water")</f>
-        <v>19.966840438464878</v>
-      </c>
-      <c r="G32" s="5">
-        <f>[1]!PropsSI("H","T",$C32,"Q",0,"Water")/1000</f>
-        <v>1085.7674588110542</v>
-      </c>
-      <c r="H32" s="15">
-        <f>[1]!PropsSI("H","T",$C32,"Q",1,"Water")/1000</f>
-        <v>2800.9330729758299</v>
+      <c r="D32" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C32,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E32" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C32,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F32" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C32,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G32" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C32,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H32" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C32,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I32" s="1"/>
     </row>
@@ -7059,25 +7002,25 @@
         <f t="shared" si="0"/>
         <v>533.15</v>
       </c>
-      <c r="D33" s="6">
-        <f>[1]!PropsSI("P","T",C33,"Q",1,"Water")/1000</f>
-        <v>4692.260992299477</v>
-      </c>
-      <c r="E33" s="7">
-        <f>[1]!PropsSI("D","T",$C33,"Q",0,"Water")</f>
-        <v>783.62569286973462</v>
-      </c>
-      <c r="F33" s="7">
-        <f>[1]!PropsSI("D","T",$C33,"Q",1,"Water")</f>
-        <v>23.711700367712318</v>
-      </c>
-      <c r="G33" s="5">
-        <f>[1]!PropsSI("H","T",$C33,"Q",0,"Water")/1000</f>
-        <v>1134.9579569891273</v>
-      </c>
-      <c r="H33" s="15">
-        <f>[1]!PropsSI("H","T",$C33,"Q",1,"Water")/1000</f>
-        <v>2796.6032203853515</v>
+      <c r="D33" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C33,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E33" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C33,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F33" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C33,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G33" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C33,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H33" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C33,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I33" s="1"/>
     </row>
@@ -7090,25 +7033,25 @@
         <f t="shared" si="0"/>
         <v>543.15</v>
       </c>
-      <c r="D34" s="6">
-        <f>[1]!PropsSI("P","T",C34,"Q",1,"Water")/1000</f>
-        <v>5502.9867830144822</v>
-      </c>
-      <c r="E34" s="7">
-        <f>[1]!PropsSI("D","T",$C34,"Q",0,"Water")</f>
-        <v>767.46116679898171</v>
-      </c>
-      <c r="F34" s="7">
-        <f>[1]!PropsSI("D","T",$C34,"Q",1,"Water")</f>
-        <v>28.073335624424267</v>
-      </c>
-      <c r="G34" s="5">
-        <f>[1]!PropsSI("H","T",$C34,"Q",0,"Water")/1000</f>
-        <v>1185.2699943566115</v>
-      </c>
-      <c r="H34" s="15">
-        <f>[1]!PropsSI("H","T",$C34,"Q",1,"Water")/1000</f>
-        <v>2789.6932193000116</v>
+      <c r="D34" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C34,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E34" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C34,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F34" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C34,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G34" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C34,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H34" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C34,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I34" s="1"/>
     </row>
@@ -7121,25 +7064,25 @@
         <f t="shared" si="0"/>
         <v>553.15</v>
       </c>
-      <c r="D35" s="6">
-        <f>[1]!PropsSI("P","T",C35,"Q",1,"Water")/1000</f>
-        <v>6416.5829095313811</v>
-      </c>
-      <c r="E35" s="7">
-        <f>[1]!PropsSI("D","T",$C35,"Q",0,"Water")</f>
-        <v>750.27516129988146</v>
-      </c>
-      <c r="F35" s="7">
-        <f>[1]!PropsSI("D","T",$C35,"Q",1,"Water")</f>
-        <v>33.164674054046102</v>
-      </c>
-      <c r="G35" s="5">
-        <f>[1]!PropsSI("H","T",$C35,"Q",0,"Water")/1000</f>
-        <v>1236.8846659592693</v>
-      </c>
-      <c r="H35" s="15">
-        <f>[1]!PropsSI("H","T",$C35,"Q",1,"Water")/1000</f>
-        <v>2779.8667305294516</v>
+      <c r="D35" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C35,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E35" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C35,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F35" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C35,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G35" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C35,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H35" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C35,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I35" s="1"/>
     </row>
@@ -7152,25 +7095,25 @@
         <f t="shared" si="0"/>
         <v>563.15</v>
       </c>
-      <c r="D36" s="6">
-        <f>[1]!PropsSI("P","T",C36,"Q",1,"Water")/1000</f>
-        <v>7441.7783444211764</v>
-      </c>
-      <c r="E36" s="7">
-        <f>[1]!PropsSI("D","T",$C36,"Q",0,"Water")</f>
-        <v>731.90519964368571</v>
-      </c>
-      <c r="F36" s="7">
-        <f>[1]!PropsSI("D","T",$C36,"Q",1,"Water")</f>
-        <v>39.131512960158567</v>
-      </c>
-      <c r="G36" s="5">
-        <f>[1]!PropsSI("H","T",$C36,"Q",0,"Water")/1000</f>
-        <v>1290.0311497479684</v>
-      </c>
-      <c r="H36" s="15">
-        <f>[1]!PropsSI("H","T",$C36,"Q",1,"Water")/1000</f>
-        <v>2766.6990506391339</v>
+      <c r="D36" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C36,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E36" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C36,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F36" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C36,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G36" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C36,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H36" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C36,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -7183,25 +7126,25 @@
         <f t="shared" si="0"/>
         <v>573.15</v>
       </c>
-      <c r="D37" s="6">
-        <f>[1]!PropsSI("P","T",C37,"Q",1,"Water")/1000</f>
-        <v>8587.9049408351511</v>
-      </c>
-      <c r="E37" s="7">
-        <f>[1]!PropsSI("D","T",$C37,"Q",0,"Water")</f>
-        <v>712.13563881961386</v>
-      </c>
-      <c r="F37" s="7">
-        <f>[1]!PropsSI("D","T",$C37,"Q",1,"Water")</f>
-        <v>46.167849523793997</v>
-      </c>
-      <c r="G37" s="5">
-        <f>[1]!PropsSI("H","T",$C37,"Q",0,"Water")/1000</f>
-        <v>1345.0079264161159</v>
-      </c>
-      <c r="H37" s="15">
-        <f>[1]!PropsSI("H","T",$C37,"Q",1,"Water")/1000</f>
-        <v>2749.638761400251</v>
+      <c r="D37" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C37,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E37" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C37,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F37" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C37,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G37" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C37,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H37" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C37,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I37" s="1"/>
     </row>
@@ -7214,25 +7157,25 @@
         <f t="shared" si="0"/>
         <v>583.15</v>
       </c>
-      <c r="D38" s="6">
-        <f>[1]!PropsSI("P","T",C38,"Q",1,"Water")/1000</f>
-        <v>9865.051211181868</v>
-      </c>
-      <c r="E38" s="7">
-        <f>[1]!PropsSI("D","T",$C38,"Q",0,"Water")</f>
-        <v>690.67154560984454</v>
-      </c>
-      <c r="F38" s="7">
-        <f>[1]!PropsSI("D","T",$C38,"Q",1,"Water")</f>
-        <v>54.541361541638288</v>
-      </c>
-      <c r="G38" s="5">
-        <f>[1]!PropsSI("H","T",$C38,"Q",0,"Water")/1000</f>
-        <v>1402.2171260009679</v>
-      </c>
-      <c r="H38" s="15">
-        <f>[1]!PropsSI("H","T",$C38,"Q",1,"Water")/1000</f>
-        <v>2727.9458789653854</v>
+      <c r="D38" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C38,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E38" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C38,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F38" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C38,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G38" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C38,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H38" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C38,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I38" s="1"/>
     </row>
@@ -7245,25 +7188,25 @@
         <f t="shared" si="0"/>
         <v>593.15</v>
       </c>
-      <c r="D39" s="6">
-        <f>[1]!PropsSI("P","T",C39,"Q",1,"Water")/1000</f>
-        <v>11284.292927464998</v>
-      </c>
-      <c r="E39" s="7">
-        <f>[1]!PropsSI("D","T",$C39,"Q",0,"Water")</f>
-        <v>667.09384803259582</v>
-      </c>
-      <c r="F39" s="7">
-        <f>[1]!PropsSI("D","T",$C39,"Q",1,"Water")</f>
-        <v>64.638432419886115</v>
-      </c>
-      <c r="G39" s="5">
-        <f>[1]!PropsSI("H","T",$C39,"Q",0,"Water")/1000</f>
-        <v>1462.2236463970921</v>
-      </c>
-      <c r="H39" s="15">
-        <f>[1]!PropsSI("H","T",$C39,"Q",1,"Water")/1000</f>
-        <v>2700.5857692409359</v>
+      <c r="D39" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C39,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E39" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C39,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F39" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C39,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G39" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C39,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H39" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C39,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I39" s="1"/>
     </row>
@@ -7276,25 +7219,25 @@
         <f t="shared" si="0"/>
         <v>603.15</v>
       </c>
-      <c r="D40" s="6">
-        <f>[1]!PropsSI("P","T",C40,"Q",1,"Water")/1000</f>
-        <v>12858.051600204844</v>
-      </c>
-      <c r="E40" s="7">
-        <f>[1]!PropsSI("D","T",$C40,"Q",0,"Water")</f>
-        <v>640.77321526639594</v>
-      </c>
-      <c r="F40" s="7">
-        <f>[1]!PropsSI("D","T",$C40,"Q",1,"Water")</f>
-        <v>77.050425987313361</v>
-      </c>
-      <c r="G40" s="5">
-        <f>[1]!PropsSI("H","T",$C40,"Q",0,"Water")/1000</f>
-        <v>1525.8683270550669</v>
-      </c>
-      <c r="H40" s="15">
-        <f>[1]!PropsSI("H","T",$C40,"Q",1,"Water")/1000</f>
-        <v>2666.0311405571688</v>
+      <c r="D40" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C40,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E40" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C40,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F40" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C40,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G40" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C40,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H40" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C40,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I40" s="1"/>
     </row>
@@ -7307,25 +7250,25 @@
         <f t="shared" si="0"/>
         <v>613.15</v>
       </c>
-      <c r="D41" s="6">
-        <f>[1]!PropsSI("P","T",C41,"Q",1,"Water")/1000</f>
-        <v>14600.677372002267</v>
-      </c>
-      <c r="E41" s="7">
-        <f>[1]!PropsSI("D","T",$C41,"Q",0,"Water")</f>
-        <v>610.66759832540311</v>
-      </c>
-      <c r="F41" s="7">
-        <f>[1]!PropsSI("D","T",$C41,"Q",1,"Water")</f>
-        <v>92.75878250741664</v>
-      </c>
-      <c r="G41" s="5">
-        <f>[1]!PropsSI("H","T",$C41,"Q",0,"Water")/1000</f>
-        <v>1594.528992236294</v>
-      </c>
-      <c r="H41" s="15">
-        <f>[1]!PropsSI("H","T",$C41,"Q",1,"Water")/1000</f>
-        <v>2621.8455755251834</v>
+      <c r="D41" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C41,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E41" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C41,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F41" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C41,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G41" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C41,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H41" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C41,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I41" s="1"/>
     </row>
@@ -7338,25 +7281,25 @@
         <f t="shared" si="0"/>
         <v>623.15</v>
       </c>
-      <c r="D42" s="6">
-        <f>[1]!PropsSI("P","T",C42,"Q",1,"Water")/1000</f>
-        <v>16529.415139051383</v>
-      </c>
-      <c r="E42" s="7">
-        <f>[1]!PropsSI("D","T",$C42,"Q",0,"Water")</f>
-        <v>574.70651653764321</v>
-      </c>
-      <c r="F42" s="7">
-        <f>[1]!PropsSI("D","T",$C42,"Q",1,"Water")</f>
-        <v>113.60561050162258</v>
-      </c>
-      <c r="G42" s="5">
-        <f>[1]!PropsSI("H","T",$C42,"Q",0,"Water")/1000</f>
-        <v>1670.8899067278082</v>
-      </c>
-      <c r="H42" s="15">
-        <f>[1]!PropsSI("H","T",$C42,"Q",1,"Water")/1000</f>
-        <v>2563.6367109445878</v>
+      <c r="D42" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C42,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E42" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C42,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F42" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C42,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G42" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C42,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H42" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C42,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I42" s="1"/>
     </row>
@@ -7369,25 +7312,25 @@
         <f t="shared" si="0"/>
         <v>633.15</v>
       </c>
-      <c r="D43" s="6">
-        <f>[1]!PropsSI("P","T",C43,"Q",1,"Water")/1000</f>
-        <v>18666.006646276372</v>
-      </c>
-      <c r="E43" s="7">
-        <f>[1]!PropsSI("D","T",$C43,"Q",0,"Water")</f>
-        <v>527.59162942229307</v>
-      </c>
-      <c r="F43" s="7">
-        <f>[1]!PropsSI("D","T",$C43,"Q",1,"Water")</f>
-        <v>143.89841140849438</v>
-      </c>
-      <c r="G43" s="5">
-        <f>[1]!PropsSI("H","T",$C43,"Q",0,"Water")/1000</f>
-        <v>1761.6646205355523</v>
-      </c>
-      <c r="H43" s="15">
-        <f>[1]!PropsSI("H","T",$C43,"Q",1,"Water")/1000</f>
-        <v>2481.4924833359378</v>
+      <c r="D43" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C43,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E43" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C43,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F43" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C43,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G43" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C43,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H43" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C43,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I43" s="1"/>
     </row>
@@ -7400,57 +7343,57 @@
         <f t="shared" si="0"/>
         <v>643.15</v>
       </c>
-      <c r="D44" s="6">
-        <f>[1]!PropsSI("P","T",C44,"Q",1,"Water")/1000</f>
-        <v>21043.563147465797</v>
-      </c>
-      <c r="E44" s="7">
-        <f>[1]!PropsSI("D","T",$C44,"Q",0,"Water")</f>
-        <v>451.42564747531435</v>
-      </c>
-      <c r="F44" s="7">
-        <f>[1]!PropsSI("D","T",$C44,"Q",1,"Water")</f>
-        <v>201.83931641741896</v>
-      </c>
-      <c r="G44" s="5">
-        <f>[1]!PropsSI("H","T",$C44,"Q",0,"Water")/1000</f>
-        <v>1890.6872488661777</v>
-      </c>
-      <c r="H44" s="15">
-        <f>[1]!PropsSI("H","T",$C44,"Q",1,"Water")/1000</f>
-        <v>2334.5182916068898</v>
+      <c r="D44" s="6" t="e">
+        <f ca="1">PropsSI("P","T",C44,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E44" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C44,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F44" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C44,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G44" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C44,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H44" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C44,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17"/>
-      <c r="B45" s="16">
-        <f>C45-273.15</f>
-        <v>373.94600000000003</v>
-      </c>
-      <c r="C45" s="41">
-        <f>[1]!Props1SI("Tcrit","Water")</f>
-        <v>647.096</v>
-      </c>
-      <c r="D45" s="6">
-        <f>[1]!Props1SI("Pcrit","Water")/1000</f>
-        <v>22064</v>
-      </c>
-      <c r="E45" s="7">
-        <f>[1]!PropsSI("D","T",$C45,"Q",0,"Water")</f>
-        <v>322.00000000000006</v>
-      </c>
-      <c r="F45" s="7">
-        <f>[1]!PropsSI("D","T",$C45,"Q",1,"Water")</f>
-        <v>322.00000000000006</v>
-      </c>
-      <c r="G45" s="5">
-        <f>[1]!PropsSI("H","T",$C45,"Q",0,"Water")/1000</f>
-        <v>2084.2562559079452</v>
-      </c>
-      <c r="H45" s="15">
-        <f>[1]!PropsSI("H","T",$C45,"Q",1,"Water")/1000</f>
-        <v>2084.2562559079452</v>
+      <c r="B45" s="16" t="e">
+        <f ca="1">C45-273.15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C45" s="41" t="e">
+        <f ca="1">Props1SI("Tcrit","Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D45" s="6" t="e">
+        <f ca="1">Props1SI("Pcrit","Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E45" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C45,"Q",0,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F45" s="7" t="e">
+        <f ca="1">PropsSI("D","T",$C45,"Q",1,"Water")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G45" s="5" t="e">
+        <f ca="1">PropsSI("H","T",$C45,"Q",0,"Water")/1000</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H45" s="15" t="e">
+        <f ca="1">PropsSI("H","T",$C45,"Q",1,"Water")/1000</f>
+        <v>#NAME?</v>
       </c>
       <c r="I45" s="1"/>
     </row>
@@ -7486,13 +7429,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" customWidth="1"/>
-    <col min="8" max="8" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="3.625" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
+    <col min="4" max="4" width="3.75" customWidth="1"/>
+    <col min="5" max="5" width="24.125" customWidth="1"/>
+    <col min="6" max="6" width="3.375" customWidth="1"/>
+    <col min="7" max="7" width="4.625" customWidth="1"/>
+    <col min="8" max="8" width="3.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -7702,9 +7645,9 @@
         <v>523</v>
       </c>
       <c r="D18" s="46"/>
-      <c r="E18" s="62">
-        <f>[1]!PropsSI(E10,E12,E13,E15,E16,E8)</f>
-        <v>2715703.752016522</v>
+      <c r="E18" s="62" t="e">
+        <f ca="1">PropsSI(E10,E12,E13,E15,E16,E8)</f>
+        <v>#NAME?</v>
       </c>
       <c r="F18" s="54"/>
       <c r="G18" s="49"/>
@@ -7766,28 +7709,28 @@
   <dimension ref="B2:DT170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="40.25" customWidth="1"/>
+    <col min="4" max="4" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.875" customWidth="1"/>
+    <col min="6" max="6" width="21.125" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.125" customWidth="1"/>
+    <col min="10" max="10" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B2" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="43" t="str">
-        <f>[1]!get_global_param_string("FluidsList")</f>
-        <v>1-Butene,Acetone,Air,Ammonia,Argon,Benzene,CarbonDioxide,CarbonMonoxide,CarbonylSulfide,cis-2-Butene,CycloHexane,Cyclopentane,CycloPropane,D4,D5,D6,Deuterium,Dichloroethane,DiethylEther,DimethylCarbonate,DimethylEther,Ethane,Ethanol,EthylBenzene,Ethylene,EthyleneOxide,Fluorine,HeavyWater,Helium,HFE143m,Hydrogen,HydrogenChloride,HydrogenSulfide,IsoButane,IsoButene,Isohexane,Isopentane,Krypton,m-Xylene,MD2M,MD3M,MD4M,MDM,Methane,Methanol,MethylLinoleate,MethylLinolenate,MethylOleate,MethylPalmitate,MethylStearate,MM,n-Butane,n-Decane,n-Dodecane,n-Heptane,n-Hexane,n-Nonane,n-Octane,n-Pentane,n-Propane,n-Undecane,Neon,Neopentane,Nitrogen,NitrousOxide,Novec649,o-Xylene,OrthoDeuterium,OrthoHydrogen,Oxygen,p-Xylene,ParaDeuterium,ParaHydrogen,Propylene,Propyne,R11,R113,R114,R115,R116,R12,R123,R1233zd(E),R1234yf,R1234ze(E),R1234ze(Z),R124,R125,R13,R134a,R13I1,R14,R141b,R142b,R143a,R152A,R161,R21,R218,R22,R227EA,R23,R236EA,R236FA,R245ca,R245fa,R32,R365MFC,R40,R404A,R407C,R41,R410A,R507A,RC318,SES36,SulfurDioxide,SulfurHexafluoride,Toluene,trans-2-Butene,Water,Xenon</v>
+      <c r="C2" s="43" t="e">
+        <f ca="1">get_global_param_string("FluidsList")</f>
+        <v>#NAME?</v>
       </c>
       <c r="D2" s="43"/>
       <c r="E2" s="43"/>

</xml_diff>